<commit_message>
cierre 28 MAR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #03  MARZO  2022/ENTRADAS OBRADOR  MaRzO     2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #03  MARZO  2022/ENTRADAS OBRADOR  MaRzO     2022.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="255">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -623,12 +623,6 @@
     <t>T-8</t>
   </si>
   <si>
-    <t>20079--</t>
-  </si>
-  <si>
-    <t>20086--</t>
-  </si>
-  <si>
     <t>T-10</t>
   </si>
   <si>
@@ -671,18 +665,6 @@
     <t>T-13</t>
   </si>
   <si>
-    <t>20091--</t>
-  </si>
-  <si>
-    <t>20104--</t>
-  </si>
-  <si>
-    <t>20116--</t>
-  </si>
-  <si>
-    <t>20122--</t>
-  </si>
-  <si>
     <t>XXXXX</t>
   </si>
   <si>
@@ -718,6 +700,99 @@
   <si>
     <t>XXXX</t>
   </si>
+  <si>
+    <t>AGROPECUARIA LA CHEMITA  248</t>
+  </si>
+  <si>
+    <t>AGROPECUARIA LA CHEMITA   250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PORCICOLA SAN BERNARDO </t>
+  </si>
+  <si>
+    <t>FOLIO CENTRAL 6946</t>
+  </si>
+  <si>
+    <t>A838</t>
+  </si>
+  <si>
+    <t>T-17</t>
+  </si>
+  <si>
+    <t>T-16</t>
+  </si>
+  <si>
+    <t>T-18</t>
+  </si>
+  <si>
+    <t>FOLIO CENTRAL 6956</t>
+  </si>
+  <si>
+    <t>A851</t>
+  </si>
+  <si>
+    <t>20079--10704</t>
+  </si>
+  <si>
+    <t>20079--3220</t>
+  </si>
+  <si>
+    <t>20086--10710</t>
+  </si>
+  <si>
+    <t>20086--3224</t>
+  </si>
+  <si>
+    <t>20091--10711</t>
+  </si>
+  <si>
+    <t>20104--4684</t>
+  </si>
+  <si>
+    <t>20104--3232</t>
+  </si>
+  <si>
+    <t>20091--8696</t>
+  </si>
+  <si>
+    <t>20132--</t>
+  </si>
+  <si>
+    <t>20143--</t>
+  </si>
+  <si>
+    <t>20161--</t>
+  </si>
+  <si>
+    <t>20169--</t>
+  </si>
+  <si>
+    <t>PULPA ESPALDILLA</t>
+  </si>
+  <si>
+    <t>FOLIO 10716</t>
+  </si>
+  <si>
+    <t>PECHO S/G</t>
+  </si>
+  <si>
+    <t>CABEZA DE LOMO</t>
+  </si>
+  <si>
+    <t>FOLIO 10710</t>
+  </si>
+  <si>
+    <t>20116--3242</t>
+  </si>
+  <si>
+    <t>20116--10726</t>
+  </si>
+  <si>
+    <t>20122--3239</t>
+  </si>
+  <si>
+    <t>20122--6729</t>
+  </si>
 </sst>
 </file>
 
@@ -730,7 +805,7 @@
     <numFmt numFmtId="166" formatCode="[$-C0A]dd\-mmm\-yy;@"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="49" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1116,6 +1191,14 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2028,7 +2111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="498">
+  <cellXfs count="512">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3212,9 +3295,6 @@
     <xf numFmtId="0" fontId="30" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3243,6 +3323,93 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="11" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3276,84 +3443,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3384,8 +3479,38 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="49" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="49" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3715,18 +3840,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="450" t="s">
+      <c r="A1" s="478" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="450"/>
-      <c r="C1" s="450"/>
-      <c r="D1" s="450"/>
-      <c r="E1" s="450"/>
-      <c r="F1" s="450"/>
-      <c r="G1" s="450"/>
-      <c r="H1" s="450"/>
-      <c r="I1" s="450"/>
-      <c r="J1" s="450"/>
+      <c r="B1" s="478"/>
+      <c r="C1" s="478"/>
+      <c r="D1" s="478"/>
+      <c r="E1" s="478"/>
+      <c r="F1" s="478"/>
+      <c r="G1" s="478"/>
+      <c r="H1" s="478"/>
+      <c r="I1" s="478"/>
+      <c r="J1" s="478"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -3740,22 +3865,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="451" t="s">
+      <c r="W1" s="479" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="452"/>
+      <c r="X1" s="480"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="450"/>
-      <c r="B2" s="450"/>
-      <c r="C2" s="450"/>
-      <c r="D2" s="450"/>
-      <c r="E2" s="450"/>
-      <c r="F2" s="450"/>
-      <c r="G2" s="450"/>
-      <c r="H2" s="450"/>
-      <c r="I2" s="450"/>
-      <c r="J2" s="450"/>
+      <c r="A2" s="478"/>
+      <c r="B2" s="478"/>
+      <c r="C2" s="478"/>
+      <c r="D2" s="478"/>
+      <c r="E2" s="478"/>
+      <c r="F2" s="478"/>
+      <c r="G2" s="478"/>
+      <c r="H2" s="478"/>
+      <c r="I2" s="478"/>
+      <c r="J2" s="478"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -3809,10 +3934,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="453" t="s">
+      <c r="O3" s="481" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="454"/>
+      <c r="P3" s="482"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -4356,7 +4481,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="455" t="s">
+      <c r="C12" s="483" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="400"/>
@@ -4420,7 +4545,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="456"/>
+      <c r="C13" s="484"/>
       <c r="D13" s="400"/>
       <c r="E13" s="401"/>
       <c r="F13" s="402">
@@ -6422,13 +6547,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="467" t="s">
+      <c r="A56" s="462" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="469" t="s">
+      <c r="C56" s="464" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -6439,7 +6564,7 @@
       <c r="G56" s="152">
         <v>44571</v>
       </c>
-      <c r="H56" s="461">
+      <c r="H56" s="466">
         <v>782</v>
       </c>
       <c r="I56" s="151">
@@ -6468,11 +6593,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="468"/>
+      <c r="A57" s="463"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="470"/>
+      <c r="C57" s="465"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -6481,7 +6606,7 @@
       <c r="G57" s="152">
         <v>44571</v>
       </c>
-      <c r="H57" s="462"/>
+      <c r="H57" s="467"/>
       <c r="I57" s="151">
         <v>319</v>
       </c>
@@ -6508,13 +6633,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="467" t="s">
+      <c r="A58" s="462" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="469" t="s">
+      <c r="C58" s="464" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="150"/>
@@ -6525,7 +6650,7 @@
       <c r="G58" s="152">
         <v>44578</v>
       </c>
-      <c r="H58" s="461">
+      <c r="H58" s="466">
         <v>810</v>
       </c>
       <c r="I58" s="151">
@@ -6544,10 +6669,10 @@
         <f t="shared" si="1"/>
         <v>75875.8</v>
       </c>
-      <c r="O58" s="463" t="s">
+      <c r="O58" s="468" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="465">
+      <c r="P58" s="489">
         <v>44606</v>
       </c>
       <c r="Q58" s="128"/>
@@ -6558,11 +6683,11 @@
       <c r="V58" s="160"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="468"/>
+      <c r="A59" s="463"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="470"/>
+      <c r="C59" s="465"/>
       <c r="D59" s="150"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151">
@@ -6571,7 +6696,7 @@
       <c r="G59" s="152">
         <v>44578</v>
       </c>
-      <c r="H59" s="462"/>
+      <c r="H59" s="467"/>
       <c r="I59" s="151">
         <v>220</v>
       </c>
@@ -6588,8 +6713,8 @@
         <f t="shared" si="1"/>
         <v>22440</v>
       </c>
-      <c r="O59" s="464"/>
-      <c r="P59" s="466"/>
+      <c r="O59" s="469"/>
+      <c r="P59" s="490"/>
       <c r="Q59" s="128"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -6598,13 +6723,13 @@
       <c r="V59" s="160"/>
     </row>
     <row r="60" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="459" t="s">
+      <c r="A60" s="487" t="s">
         <v>41</v>
       </c>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="457" t="s">
+      <c r="C60" s="485" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="163"/>
@@ -6618,7 +6743,7 @@
       <c r="G60" s="152">
         <v>44585</v>
       </c>
-      <c r="H60" s="461">
+      <c r="H60" s="466">
         <v>800</v>
       </c>
       <c r="I60" s="151">
@@ -6637,10 +6762,10 @@
         <f t="shared" si="1"/>
         <v>151187.4</v>
       </c>
-      <c r="O60" s="463" t="s">
+      <c r="O60" s="468" t="s">
         <v>59</v>
       </c>
-      <c r="P60" s="465">
+      <c r="P60" s="489">
         <v>44594</v>
       </c>
       <c r="Q60" s="164"/>
@@ -6653,11 +6778,11 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="460"/>
+      <c r="A61" s="488"/>
       <c r="B61" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="458"/>
+      <c r="C61" s="486"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -6669,7 +6794,7 @@
       <c r="G61" s="152">
         <v>44585</v>
       </c>
-      <c r="H61" s="462"/>
+      <c r="H61" s="467"/>
       <c r="I61" s="151">
         <v>231.6</v>
       </c>
@@ -6686,8 +6811,8 @@
         <f t="shared" si="1"/>
         <v>23623.200000000001</v>
       </c>
-      <c r="O61" s="464"/>
-      <c r="P61" s="466"/>
+      <c r="O61" s="469"/>
+      <c r="P61" s="490"/>
       <c r="Q61" s="164"/>
       <c r="R61" s="129"/>
       <c r="S61" s="92"/>
@@ -6753,7 +6878,7 @@
       <c r="B63" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="483"/>
+      <c r="C63" s="456"/>
       <c r="D63" s="163"/>
       <c r="E63" s="40">
         <f t="shared" si="2"/>
@@ -6761,7 +6886,7 @@
       </c>
       <c r="F63" s="151"/>
       <c r="G63" s="152"/>
-      <c r="H63" s="485"/>
+      <c r="H63" s="458"/>
       <c r="I63" s="151"/>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
@@ -6790,7 +6915,7 @@
       <c r="B64" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="484"/>
+      <c r="C64" s="457"/>
       <c r="D64" s="168"/>
       <c r="E64" s="40">
         <f t="shared" si="2"/>
@@ -6798,7 +6923,7 @@
       </c>
       <c r="F64" s="151"/>
       <c r="G64" s="152"/>
-      <c r="H64" s="486"/>
+      <c r="H64" s="459"/>
       <c r="I64" s="151"/>
       <c r="J64" s="45">
         <f t="shared" si="0"/>
@@ -6976,8 +7101,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O68" s="475"/>
-      <c r="P68" s="481"/>
+      <c r="O68" s="460"/>
+      <c r="P68" s="454"/>
       <c r="Q68" s="164"/>
       <c r="R68" s="129"/>
       <c r="S68" s="180"/>
@@ -7011,8 +7136,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O69" s="476"/>
-      <c r="P69" s="482"/>
+      <c r="O69" s="461"/>
+      <c r="P69" s="455"/>
       <c r="Q69" s="164"/>
       <c r="R69" s="129"/>
       <c r="S69" s="180"/>
@@ -7502,8 +7627,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="475"/>
-      <c r="P82" s="477"/>
+      <c r="O82" s="460"/>
+      <c r="P82" s="474"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="129"/>
       <c r="S82" s="180"/>
@@ -7535,8 +7660,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="476"/>
-      <c r="P83" s="478"/>
+      <c r="O83" s="461"/>
+      <c r="P83" s="475"/>
       <c r="Q83" s="164"/>
       <c r="R83" s="129"/>
       <c r="S83" s="180"/>
@@ -7568,8 +7693,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O84" s="475"/>
-      <c r="P84" s="477"/>
+      <c r="O84" s="460"/>
+      <c r="P84" s="474"/>
       <c r="Q84" s="164"/>
       <c r="R84" s="158"/>
       <c r="S84" s="180"/>
@@ -7601,8 +7726,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O85" s="476"/>
-      <c r="P85" s="478"/>
+      <c r="O85" s="461"/>
+      <c r="P85" s="475"/>
       <c r="Q85" s="164"/>
       <c r="R85" s="158"/>
       <c r="S85" s="180"/>
@@ -7760,8 +7885,8 @@
         <v>0</v>
       </c>
       <c r="K90" s="100"/>
-      <c r="L90" s="479"/>
-      <c r="M90" s="480"/>
+      <c r="L90" s="476"/>
+      <c r="M90" s="477"/>
       <c r="N90" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7793,8 +7918,8 @@
         <v>0</v>
       </c>
       <c r="K91" s="100"/>
-      <c r="L91" s="479"/>
-      <c r="M91" s="480"/>
+      <c r="L91" s="476"/>
+      <c r="M91" s="477"/>
       <c r="N91" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -7997,8 +8122,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O97" s="475"/>
-      <c r="P97" s="471"/>
+      <c r="O97" s="460"/>
+      <c r="P97" s="470"/>
       <c r="Q97" s="164"/>
       <c r="R97" s="129"/>
       <c r="S97" s="180"/>
@@ -8030,8 +8155,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O98" s="476"/>
-      <c r="P98" s="472"/>
+      <c r="O98" s="461"/>
+      <c r="P98" s="471"/>
       <c r="Q98" s="164"/>
       <c r="R98" s="129"/>
       <c r="S98" s="180"/>
@@ -13423,11 +13548,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F262" s="473" t="s">
+      <c r="F262" s="472" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="473"/>
-      <c r="H262" s="474"/>
+      <c r="G262" s="472"/>
+      <c r="H262" s="473"/>
       <c r="I262" s="317">
         <f>SUM(I4:I261)</f>
         <v>426245.47000000003</v>
@@ -14001,22 +14126,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
-    <mergeCell ref="P97:P98"/>
-    <mergeCell ref="F262:H262"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="L90:M91"/>
-    <mergeCell ref="O97:O98"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
@@ -14030,6 +14139,22 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="P58:P59"/>
+    <mergeCell ref="P97:P98"/>
+    <mergeCell ref="F262:H262"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="L90:M91"/>
+    <mergeCell ref="O97:O98"/>
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14044,10 +14169,10 @@
   <dimension ref="A1:X292"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="O21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O31" sqref="O31"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14076,49 +14201,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="450" t="s">
+      <c r="A1" s="478" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="450"/>
-      <c r="C1" s="450"/>
-      <c r="D1" s="450"/>
-      <c r="E1" s="450"/>
-      <c r="F1" s="450"/>
-      <c r="G1" s="450"/>
-      <c r="H1" s="450"/>
-      <c r="I1" s="450"/>
-      <c r="J1" s="450"/>
+      <c r="B1" s="478"/>
+      <c r="C1" s="478"/>
+      <c r="D1" s="478"/>
+      <c r="E1" s="478"/>
+      <c r="F1" s="478"/>
+      <c r="G1" s="478"/>
+      <c r="H1" s="478"/>
+      <c r="I1" s="478"/>
+      <c r="J1" s="478"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="493" t="s">
+      <c r="S1" s="497" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="493"/>
+      <c r="T1" s="497"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="451" t="s">
+      <c r="W1" s="479" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="452"/>
+      <c r="X1" s="480"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="450"/>
-      <c r="B2" s="450"/>
-      <c r="C2" s="450"/>
-      <c r="D2" s="450"/>
-      <c r="E2" s="450"/>
-      <c r="F2" s="450"/>
-      <c r="G2" s="450"/>
-      <c r="H2" s="450"/>
-      <c r="I2" s="450"/>
-      <c r="J2" s="450"/>
+      <c r="A2" s="478"/>
+      <c r="B2" s="478"/>
+      <c r="C2" s="478"/>
+      <c r="D2" s="478"/>
+      <c r="E2" s="478"/>
+      <c r="F2" s="478"/>
+      <c r="G2" s="478"/>
+      <c r="H2" s="478"/>
+      <c r="I2" s="478"/>
+      <c r="J2" s="478"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -14126,8 +14251,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="494"/>
-      <c r="T2" s="494"/>
+      <c r="S2" s="498"/>
+      <c r="T2" s="498"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -14172,10 +14297,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="453" t="s">
+      <c r="O3" s="481" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="454"/>
+      <c r="P3" s="482"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -14215,7 +14340,7 @@
       <c r="G4" s="42">
         <v>44594</v>
       </c>
-      <c r="H4" s="446" t="s">
+      <c r="H4" s="445" t="s">
         <v>138</v>
       </c>
       <c r="I4" s="409">
@@ -15312,7 +15437,7 @@
         <v>44610</v>
       </c>
       <c r="H22" s="410" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I22" s="411">
         <f>22560-112.8</f>
@@ -15377,7 +15502,7 @@
         <v>44610</v>
       </c>
       <c r="H23" s="410" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I23" s="411">
         <v>5550</v>
@@ -15441,7 +15566,7 @@
         <v>44612</v>
       </c>
       <c r="H24" s="410" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I24" s="411">
         <v>22250</v>
@@ -15505,7 +15630,7 @@
         <v>44612</v>
       </c>
       <c r="H25" s="410" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I25" s="411">
         <v>5400</v>
@@ -15569,7 +15694,7 @@
         <v>44615</v>
       </c>
       <c r="H26" s="410" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I26" s="411">
         <f>21065-105.33</f>
@@ -15634,7 +15759,7 @@
         <v>44615</v>
       </c>
       <c r="H27" s="410" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I27" s="411">
         <v>5485</v>
@@ -15698,7 +15823,7 @@
         <v>44617</v>
       </c>
       <c r="H28" s="410" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="I28" s="411">
         <v>21600</v>
@@ -15717,7 +15842,7 @@
         <v>702000</v>
       </c>
       <c r="O28" s="417" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="P28" s="418">
         <v>44631</v>
@@ -15762,7 +15887,7 @@
         <v>44617</v>
       </c>
       <c r="H29" s="410" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="I29" s="411">
         <v>5455</v>
@@ -15824,7 +15949,7 @@
         <v>44619</v>
       </c>
       <c r="H30" s="410" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="I30" s="411">
         <v>21935</v>
@@ -15848,10 +15973,10 @@
       <c r="P30" s="418">
         <v>44634</v>
       </c>
-      <c r="Q30" s="444">
+      <c r="Q30" s="443">
         <v>25140</v>
       </c>
-      <c r="R30" s="445">
+      <c r="R30" s="444">
         <v>44627</v>
       </c>
       <c r="S30" s="91">
@@ -15886,7 +16011,7 @@
         <v>44619</v>
       </c>
       <c r="H31" s="63" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="I31" s="64">
         <v>5470</v>
@@ -15910,10 +16035,10 @@
       <c r="P31" s="418">
         <v>44634</v>
       </c>
-      <c r="Q31" s="444">
-        <v>0</v>
-      </c>
-      <c r="R31" s="445">
+      <c r="Q31" s="443">
+        <v>0</v>
+      </c>
+      <c r="R31" s="444">
         <v>44627</v>
       </c>
       <c r="S31" s="91">
@@ -16697,13 +16822,13 @@
       <c r="V54" s="160"/>
     </row>
     <row r="55" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="495" t="s">
+      <c r="A55" s="499" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="469" t="s">
+      <c r="C55" s="464" t="s">
         <v>160</v>
       </c>
       <c r="D55" s="150"/>
@@ -16714,7 +16839,7 @@
       <c r="G55" s="152">
         <v>44599</v>
       </c>
-      <c r="H55" s="485" t="s">
+      <c r="H55" s="458" t="s">
         <v>161</v>
       </c>
       <c r="I55" s="151">
@@ -16743,11 +16868,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="496"/>
+      <c r="A56" s="500"/>
       <c r="B56" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="470"/>
+      <c r="C56" s="465"/>
       <c r="D56" s="163"/>
       <c r="E56" s="40"/>
       <c r="F56" s="151">
@@ -16756,7 +16881,7 @@
       <c r="G56" s="152">
         <v>44599</v>
       </c>
-      <c r="H56" s="486"/>
+      <c r="H56" s="459"/>
       <c r="I56" s="151">
         <v>194.4</v>
       </c>
@@ -16785,13 +16910,13 @@
       <c r="X56"/>
     </row>
     <row r="57" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="487" t="s">
+      <c r="A57" s="491" t="s">
         <v>41</v>
       </c>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="489" t="s">
+      <c r="C57" s="493" t="s">
         <v>162</v>
       </c>
       <c r="D57" s="165"/>
@@ -16802,7 +16927,7 @@
       <c r="G57" s="152">
         <v>44606</v>
       </c>
-      <c r="H57" s="485" t="s">
+      <c r="H57" s="458" t="s">
         <v>163</v>
       </c>
       <c r="I57" s="151">
@@ -16821,10 +16946,10 @@
         <f t="shared" si="1"/>
         <v>35776</v>
       </c>
-      <c r="O57" s="475" t="s">
+      <c r="O57" s="460" t="s">
         <v>59</v>
       </c>
-      <c r="P57" s="481">
+      <c r="P57" s="454">
         <v>44620</v>
       </c>
       <c r="Q57" s="164"/>
@@ -16835,11 +16960,11 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="488"/>
+      <c r="A58" s="492"/>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="490"/>
+      <c r="C58" s="494"/>
       <c r="D58" s="165"/>
       <c r="E58" s="40"/>
       <c r="F58" s="151">
@@ -16848,7 +16973,7 @@
       <c r="G58" s="152">
         <v>44606</v>
       </c>
-      <c r="H58" s="486"/>
+      <c r="H58" s="459"/>
       <c r="I58" s="151">
         <v>627.60209999999995</v>
       </c>
@@ -16865,8 +16990,8 @@
         <f t="shared" si="1"/>
         <v>58366.995299999995</v>
       </c>
-      <c r="O58" s="491"/>
-      <c r="P58" s="492"/>
+      <c r="O58" s="495"/>
+      <c r="P58" s="496"/>
       <c r="Q58" s="164"/>
       <c r="R58" s="129"/>
       <c r="S58" s="92"/>
@@ -16874,31 +16999,49 @@
       <c r="U58" s="53"/>
       <c r="V58" s="54"/>
     </row>
-    <row r="59" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="497"/>
+    <row r="59" spans="1:24" s="161" customFormat="1" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="449" t="s">
+        <v>41</v>
+      </c>
       <c r="B59" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="483"/>
+      <c r="C59" s="451" t="s">
+        <v>227</v>
+      </c>
       <c r="D59" s="163"/>
       <c r="E59" s="40"/>
-      <c r="F59" s="151"/>
-      <c r="G59" s="152"/>
-      <c r="H59" s="485"/>
-      <c r="I59" s="151"/>
+      <c r="F59" s="151">
+        <v>1544.2</v>
+      </c>
+      <c r="G59" s="152">
+        <v>44613</v>
+      </c>
+      <c r="H59" s="458" t="s">
+        <v>228</v>
+      </c>
+      <c r="I59" s="151">
+        <v>1544.2</v>
+      </c>
       <c r="J59" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K59" s="46"/>
+      <c r="K59" s="46">
+        <v>96</v>
+      </c>
       <c r="L59" s="65"/>
       <c r="M59" s="65"/>
       <c r="N59" s="154">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O59" s="164"/>
-      <c r="P59" s="62"/>
+        <v>148243.20000000001</v>
+      </c>
+      <c r="O59" s="414" t="s">
+        <v>59</v>
+      </c>
+      <c r="P59" s="453">
+        <v>44637</v>
+      </c>
       <c r="Q59" s="167"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -16909,16 +17052,16 @@
       <c r="X59"/>
     </row>
     <row r="60" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="460"/>
+      <c r="A60" s="450"/>
       <c r="B60" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="484"/>
+      <c r="C60" s="452"/>
       <c r="D60" s="168"/>
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="486"/>
+      <c r="H60" s="459"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -17121,28 +17264,48 @@
       <c r="V64" s="54"/>
     </row>
     <row r="65" spans="1:22" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A65" s="80"/>
-      <c r="B65" s="178"/>
-      <c r="C65" s="183"/>
+      <c r="A65" s="80" t="s">
+        <v>106</v>
+      </c>
+      <c r="B65" s="178" t="s">
+        <v>249</v>
+      </c>
+      <c r="C65" s="183" t="s">
+        <v>250</v>
+      </c>
       <c r="D65" s="171"/>
       <c r="E65" s="60"/>
-      <c r="F65" s="151"/>
-      <c r="G65" s="152"/>
-      <c r="H65" s="388"/>
-      <c r="I65" s="151"/>
+      <c r="F65" s="151">
+        <v>282.8</v>
+      </c>
+      <c r="G65" s="152">
+        <v>44620</v>
+      </c>
+      <c r="H65" s="153">
+        <v>37140</v>
+      </c>
+      <c r="I65" s="151">
+        <v>282.8</v>
+      </c>
       <c r="J65" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K65" s="166"/>
+      <c r="K65" s="166">
+        <v>65</v>
+      </c>
       <c r="L65" s="99"/>
       <c r="M65" s="99"/>
       <c r="N65" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O65" s="475"/>
-      <c r="P65" s="481"/>
+        <v>18382</v>
+      </c>
+      <c r="O65" s="510" t="s">
+        <v>61</v>
+      </c>
+      <c r="P65" s="511">
+        <v>44643</v>
+      </c>
       <c r="Q65" s="164"/>
       <c r="R65" s="129"/>
       <c r="S65" s="180"/>
@@ -17171,8 +17334,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O66" s="476"/>
-      <c r="P66" s="482"/>
+      <c r="O66" s="172"/>
+      <c r="P66" s="42"/>
       <c r="Q66" s="164"/>
       <c r="R66" s="129"/>
       <c r="S66" s="180"/>
@@ -17561,8 +17724,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="475"/>
-      <c r="P79" s="477"/>
+      <c r="O79" s="460"/>
+      <c r="P79" s="474"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -17591,8 +17754,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="476"/>
-      <c r="P80" s="478"/>
+      <c r="O80" s="461"/>
+      <c r="P80" s="475"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -17621,8 +17784,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="475"/>
-      <c r="P81" s="477"/>
+      <c r="O81" s="460"/>
+      <c r="P81" s="474"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -17654,8 +17817,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="476"/>
-      <c r="P82" s="478"/>
+      <c r="O82" s="461"/>
+      <c r="P82" s="475"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -17813,8 +17976,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="479"/>
-      <c r="M87" s="480"/>
+      <c r="L87" s="476"/>
+      <c r="M87" s="477"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -17846,8 +18009,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="479"/>
-      <c r="M88" s="480"/>
+      <c r="L88" s="476"/>
+      <c r="M88" s="477"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -18050,8 +18213,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="475"/>
-      <c r="P94" s="471"/>
+      <c r="O94" s="460"/>
+      <c r="P94" s="470"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -18083,8 +18246,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="476"/>
-      <c r="P95" s="472"/>
+      <c r="O95" s="461"/>
+      <c r="P95" s="471"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -23476,14 +23639,14 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="473" t="s">
+      <c r="F259" s="472" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="473"/>
-      <c r="H259" s="474"/>
+      <c r="G259" s="472"/>
+      <c r="H259" s="473"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
-        <v>385380.97210000001</v>
+        <v>387207.97210000001</v>
       </c>
       <c r="J259" s="318"/>
       <c r="K259" s="314"/>
@@ -23582,7 +23745,7 @@
       <c r="M263" s="336"/>
       <c r="N263" s="337">
         <f>SUM(N4:N262)</f>
-        <v>13093365.9353</v>
+        <v>13259991.135299999</v>
       </c>
       <c r="O263" s="338"/>
       <c r="Q263" s="339">
@@ -23642,7 +23805,7 @@
       <c r="M266" s="352"/>
       <c r="N266" s="353">
         <f>V263+S263+Q263+N263+L263</f>
-        <v>13529625.9353</v>
+        <v>13696251.135299999</v>
       </c>
       <c r="O266" s="354"/>
       <c r="R266" s="324"/>
@@ -23800,7 +23963,7 @@
       <c r="E280" s="367"/>
       <c r="F280" s="368"/>
       <c r="G280" s="369"/>
-      <c r="H280" s="449"/>
+      <c r="H280" s="448"/>
       <c r="I280" s="371"/>
       <c r="J280"/>
       <c r="K280"/>
@@ -23820,7 +23983,7 @@
       <c r="E281" s="367"/>
       <c r="F281" s="368"/>
       <c r="G281" s="369"/>
-      <c r="H281" s="449"/>
+      <c r="H281" s="448"/>
       <c r="I281" s="371"/>
       <c r="J281"/>
       <c r="K281"/>
@@ -23840,7 +24003,7 @@
       <c r="E282" s="367"/>
       <c r="F282" s="368"/>
       <c r="G282" s="369"/>
-      <c r="H282" s="449"/>
+      <c r="H282" s="448"/>
       <c r="I282" s="371"/>
       <c r="J282"/>
       <c r="K282"/>
@@ -23860,7 +24023,7 @@
       <c r="E283" s="367"/>
       <c r="F283" s="368"/>
       <c r="G283" s="369"/>
-      <c r="H283" s="449"/>
+      <c r="H283" s="448"/>
       <c r="I283" s="371"/>
       <c r="J283"/>
       <c r="K283"/>
@@ -23880,7 +24043,7 @@
       <c r="E284" s="367"/>
       <c r="F284" s="368"/>
       <c r="G284" s="369"/>
-      <c r="H284" s="449"/>
+      <c r="H284" s="448"/>
       <c r="I284" s="371"/>
       <c r="J284"/>
       <c r="K284"/>
@@ -23900,7 +24063,7 @@
       <c r="E285" s="367"/>
       <c r="F285" s="368"/>
       <c r="G285" s="369"/>
-      <c r="H285" s="449"/>
+      <c r="H285" s="448"/>
       <c r="I285" s="371"/>
       <c r="J285"/>
       <c r="K285"/>
@@ -23920,7 +24083,7 @@
       <c r="E286" s="367"/>
       <c r="F286" s="368"/>
       <c r="G286" s="369"/>
-      <c r="H286" s="449"/>
+      <c r="H286" s="448"/>
       <c r="I286" s="371"/>
       <c r="J286"/>
       <c r="K286"/>
@@ -23940,7 +24103,7 @@
       <c r="E287" s="367"/>
       <c r="F287" s="368"/>
       <c r="G287" s="369"/>
-      <c r="H287" s="449"/>
+      <c r="H287" s="448"/>
       <c r="I287" s="371"/>
       <c r="J287"/>
       <c r="K287"/>
@@ -23960,7 +24123,7 @@
       <c r="E288" s="367"/>
       <c r="F288" s="368"/>
       <c r="G288" s="369"/>
-      <c r="H288" s="449"/>
+      <c r="H288" s="448"/>
       <c r="I288" s="371"/>
       <c r="J288"/>
       <c r="K288"/>
@@ -23980,7 +24143,7 @@
       <c r="E289" s="367"/>
       <c r="F289" s="368"/>
       <c r="G289" s="369"/>
-      <c r="H289" s="449"/>
+      <c r="H289" s="448"/>
       <c r="I289" s="371"/>
       <c r="J289"/>
       <c r="K289"/>
@@ -24000,7 +24163,7 @@
       <c r="E290" s="367"/>
       <c r="F290" s="368"/>
       <c r="G290" s="369"/>
-      <c r="H290" s="449"/>
+      <c r="H290" s="448"/>
       <c r="I290" s="371"/>
       <c r="J290"/>
       <c r="K290"/>
@@ -24020,7 +24183,7 @@
       <c r="E291" s="367"/>
       <c r="F291" s="368"/>
       <c r="G291" s="369"/>
-      <c r="H291" s="449"/>
+      <c r="H291" s="448"/>
       <c r="I291" s="371"/>
       <c r="J291"/>
       <c r="K291"/>
@@ -24040,7 +24203,7 @@
       <c r="E292" s="367"/>
       <c r="F292" s="368"/>
       <c r="G292" s="369"/>
-      <c r="H292" s="449"/>
+      <c r="H292" s="448"/>
       <c r="I292" s="371"/>
       <c r="J292"/>
       <c r="K292"/>
@@ -24053,15 +24216,13 @@
       <c r="V292"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="P65:P66"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="O65:O66"/>
+  <mergeCells count="21">
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="A57:A58"/>
@@ -24073,12 +24234,10 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="H55:H56"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="H59:H60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -24093,10 +24252,10 @@
   <dimension ref="A1:X292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="S4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="M15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T13" sqref="T13"/>
+      <selection pane="bottomRight" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -24125,49 +24284,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="450" t="s">
+      <c r="A1" s="478" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="450"/>
-      <c r="C1" s="450"/>
-      <c r="D1" s="450"/>
-      <c r="E1" s="450"/>
-      <c r="F1" s="450"/>
-      <c r="G1" s="450"/>
-      <c r="H1" s="450"/>
-      <c r="I1" s="450"/>
-      <c r="J1" s="450"/>
+      <c r="B1" s="478"/>
+      <c r="C1" s="478"/>
+      <c r="D1" s="478"/>
+      <c r="E1" s="478"/>
+      <c r="F1" s="478"/>
+      <c r="G1" s="478"/>
+      <c r="H1" s="478"/>
+      <c r="I1" s="478"/>
+      <c r="J1" s="478"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="493" t="s">
+      <c r="S1" s="497" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="493"/>
+      <c r="T1" s="497"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="451" t="s">
+      <c r="W1" s="479" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="452"/>
+      <c r="X1" s="480"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="450"/>
-      <c r="B2" s="450"/>
-      <c r="C2" s="450"/>
-      <c r="D2" s="450"/>
-      <c r="E2" s="450"/>
-      <c r="F2" s="450"/>
-      <c r="G2" s="450"/>
-      <c r="H2" s="450"/>
-      <c r="I2" s="450"/>
-      <c r="J2" s="450"/>
+      <c r="A2" s="478"/>
+      <c r="B2" s="478"/>
+      <c r="C2" s="478"/>
+      <c r="D2" s="478"/>
+      <c r="E2" s="478"/>
+      <c r="F2" s="478"/>
+      <c r="G2" s="478"/>
+      <c r="H2" s="478"/>
+      <c r="I2" s="478"/>
+      <c r="J2" s="478"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -24175,8 +24334,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="494"/>
-      <c r="T2" s="494"/>
+      <c r="S2" s="498"/>
+      <c r="T2" s="498"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -24221,10 +24380,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="453" t="s">
+      <c r="O3" s="481" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="454"/>
+      <c r="P3" s="482"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -24263,7 +24422,7 @@
         <v>44621</v>
       </c>
       <c r="H4" s="433" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="I4" s="409">
         <v>24020</v>
@@ -24321,7 +24480,7 @@
         <v>44621</v>
       </c>
       <c r="H5" s="410" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="I5" s="411">
         <v>5340</v>
@@ -24379,7 +24538,7 @@
         <v>44623</v>
       </c>
       <c r="H6" s="410" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="I6" s="411">
         <v>22575</v>
@@ -24389,16 +24548,20 @@
         <v>605</v>
       </c>
       <c r="K6" s="46">
-        <v>332</v>
+        <v>32</v>
       </c>
       <c r="L6" s="65"/>
       <c r="M6" s="65"/>
       <c r="N6" s="48">
         <f t="shared" si="1"/>
-        <v>7494900</v>
-      </c>
-      <c r="O6" s="395"/>
-      <c r="P6" s="396"/>
+        <v>722400</v>
+      </c>
+      <c r="O6" s="395" t="s">
+        <v>61</v>
+      </c>
+      <c r="P6" s="396">
+        <v>44637</v>
+      </c>
       <c r="Q6" s="66">
         <v>25140</v>
       </c>
@@ -24433,7 +24596,7 @@
         <v>44623</v>
       </c>
       <c r="H7" s="410" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
       <c r="I7" s="411">
         <v>5615</v>
@@ -24451,8 +24614,12 @@
         <f t="shared" si="1"/>
         <v>179680</v>
       </c>
-      <c r="O7" s="395"/>
-      <c r="P7" s="396"/>
+      <c r="O7" s="395" t="s">
+        <v>61</v>
+      </c>
+      <c r="P7" s="396">
+        <v>44637</v>
+      </c>
       <c r="Q7" s="66">
         <v>0</v>
       </c>
@@ -24487,7 +24654,7 @@
         <v>44624</v>
       </c>
       <c r="H8" s="410" t="s">
-        <v>199</v>
+        <v>236</v>
       </c>
       <c r="I8" s="411">
         <v>21960</v>
@@ -24505,8 +24672,12 @@
         <f t="shared" si="1"/>
         <v>702720</v>
       </c>
-      <c r="O8" s="89"/>
-      <c r="P8" s="90"/>
+      <c r="O8" s="89" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" s="90">
+        <v>44638</v>
+      </c>
       <c r="Q8" s="66">
         <v>25360</v>
       </c>
@@ -24541,7 +24712,7 @@
         <v>44624</v>
       </c>
       <c r="H9" s="410" t="s">
-        <v>199</v>
+        <v>237</v>
       </c>
       <c r="I9" s="411">
         <v>5270</v>
@@ -24559,8 +24730,12 @@
         <f t="shared" si="1"/>
         <v>168640</v>
       </c>
-      <c r="O9" s="89"/>
-      <c r="P9" s="90"/>
+      <c r="O9" s="89" t="s">
+        <v>61</v>
+      </c>
+      <c r="P9" s="90">
+        <v>44638</v>
+      </c>
       <c r="Q9" s="66">
         <v>0</v>
       </c>
@@ -24578,7 +24753,7 @@
       <c r="W9" s="53"/>
       <c r="X9" s="70"/>
     </row>
-    <row r="10" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="71" t="s">
         <v>20</v>
       </c>
@@ -24595,7 +24770,7 @@
         <v>44626</v>
       </c>
       <c r="H10" s="410" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="I10" s="411">
         <v>22475</v>
@@ -24613,8 +24788,12 @@
         <f t="shared" si="1"/>
         <v>719200</v>
       </c>
-      <c r="O10" s="397"/>
-      <c r="P10" s="398"/>
+      <c r="O10" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P10" s="398">
+        <v>44642</v>
+      </c>
       <c r="Q10" s="66">
         <v>25140</v>
       </c>
@@ -24625,7 +24804,7 @@
         <v>11200</v>
       </c>
       <c r="T10" s="52" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="U10" s="53"/>
       <c r="V10" s="54"/>
@@ -24649,7 +24828,7 @@
         <v>44626</v>
       </c>
       <c r="H11" s="410" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="I11" s="411">
         <v>5515</v>
@@ -24667,8 +24846,12 @@
         <f t="shared" si="1"/>
         <v>176480</v>
       </c>
-      <c r="O11" s="397"/>
-      <c r="P11" s="398"/>
+      <c r="O11" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" s="398">
+        <v>44642</v>
+      </c>
       <c r="Q11" s="66">
         <v>0</v>
       </c>
@@ -24679,7 +24862,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="52" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="U11" s="53"/>
       <c r="V11" s="54"/>
@@ -24687,11 +24870,11 @@
       <c r="X11" s="70"/>
     </row>
     <row r="12" spans="1:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="448" t="s">
+      <c r="A12" s="447" t="s">
         <v>106</v>
       </c>
       <c r="B12" s="58" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C12" s="431"/>
       <c r="D12" s="60"/>
@@ -24702,7 +24885,9 @@
       <c r="G12" s="62">
         <v>44628</v>
       </c>
-      <c r="H12" s="447"/>
+      <c r="H12" s="446">
+        <v>37237</v>
+      </c>
       <c r="I12" s="411">
         <v>12480</v>
       </c>
@@ -24719,19 +24904,23 @@
         <f t="shared" si="1"/>
         <v>546624</v>
       </c>
-      <c r="O12" s="397"/>
-      <c r="P12" s="398"/>
+      <c r="O12" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P12" s="398">
+        <v>44643</v>
+      </c>
       <c r="Q12" s="66">
         <v>0</v>
       </c>
       <c r="R12" s="67" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S12" s="51">
         <v>0</v>
       </c>
       <c r="T12" s="52" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="U12" s="53"/>
       <c r="V12" s="54"/>
@@ -24740,7 +24929,7 @@
     </row>
     <row r="13" spans="1:24" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="71" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B13" s="58" t="s">
         <v>52</v>
@@ -24755,7 +24944,7 @@
         <v>44628</v>
       </c>
       <c r="H13" s="410" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="I13" s="411">
         <v>22675</v>
@@ -24773,8 +24962,12 @@
         <f t="shared" si="1"/>
         <v>725600</v>
       </c>
-      <c r="O13" s="397"/>
-      <c r="P13" s="398"/>
+      <c r="O13" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P13" s="398">
+        <v>44642</v>
+      </c>
       <c r="Q13" s="66">
         <v>24940</v>
       </c>
@@ -24785,7 +24978,7 @@
         <v>11200</v>
       </c>
       <c r="T13" s="52" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="U13" s="53"/>
       <c r="V13" s="54"/>
@@ -24809,7 +25002,7 @@
         <v>44628</v>
       </c>
       <c r="H14" s="410" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="I14" s="411">
         <v>5600</v>
@@ -24827,8 +25020,12 @@
         <f t="shared" si="1"/>
         <v>179200</v>
       </c>
-      <c r="O14" s="397"/>
-      <c r="P14" s="398"/>
+      <c r="O14" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P14" s="398">
+        <v>44642</v>
+      </c>
       <c r="Q14" s="66">
         <v>0</v>
       </c>
@@ -24839,16 +25036,16 @@
         <v>0</v>
       </c>
       <c r="T14" s="52" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="U14" s="53"/>
       <c r="V14" s="54"/>
       <c r="W14" s="53"/>
       <c r="X14" s="70"/>
     </row>
-    <row r="15" spans="1:24" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="73" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B15" s="58" t="s">
         <v>72</v>
@@ -24863,7 +25060,7 @@
         <v>44630</v>
       </c>
       <c r="H15" s="410" t="s">
-        <v>216</v>
+        <v>252</v>
       </c>
       <c r="I15" s="411">
         <v>22670</v>
@@ -24881,8 +25078,12 @@
         <f t="shared" si="1"/>
         <v>725440</v>
       </c>
-      <c r="O15" s="397"/>
-      <c r="P15" s="398"/>
+      <c r="O15" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P15" s="398">
+        <v>44644</v>
+      </c>
       <c r="Q15" s="66">
         <v>23140</v>
       </c>
@@ -24893,7 +25094,7 @@
         <v>11200</v>
       </c>
       <c r="T15" s="92" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="U15" s="53"/>
       <c r="V15" s="54"/>
@@ -24905,7 +25106,7 @@
         <v>105</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C16" s="74"/>
       <c r="D16" s="60"/>
@@ -24917,7 +25118,7 @@
         <v>44630</v>
       </c>
       <c r="H16" s="410" t="s">
-        <v>216</v>
+        <v>251</v>
       </c>
       <c r="I16" s="411">
         <v>3295</v>
@@ -24935,8 +25136,12 @@
         <f t="shared" si="1"/>
         <v>105440</v>
       </c>
-      <c r="O16" s="397"/>
-      <c r="P16" s="398"/>
+      <c r="O16" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P16" s="398">
+        <v>44644</v>
+      </c>
       <c r="Q16" s="66">
         <v>0</v>
       </c>
@@ -24947,7 +25152,7 @@
         <v>0</v>
       </c>
       <c r="T16" s="92" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="U16" s="53"/>
       <c r="V16" s="54"/>
@@ -24956,7 +25161,7 @@
     </row>
     <row r="17" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="75" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B17" s="58" t="s">
         <v>72</v>
@@ -24971,7 +25176,7 @@
         <v>44631</v>
       </c>
       <c r="H17" s="410" t="s">
-        <v>217</v>
+        <v>254</v>
       </c>
       <c r="I17" s="411">
         <v>23900</v>
@@ -24989,8 +25194,12 @@
         <f t="shared" si="1"/>
         <v>764800</v>
       </c>
-      <c r="O17" s="397"/>
-      <c r="P17" s="398"/>
+      <c r="O17" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P17" s="398">
+        <v>44645</v>
+      </c>
       <c r="Q17" s="66">
         <v>25240</v>
       </c>
@@ -25001,7 +25210,7 @@
         <v>11200</v>
       </c>
       <c r="T17" s="92" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="U17" s="53"/>
       <c r="V17" s="54"/>
@@ -25025,7 +25234,7 @@
         <v>44631</v>
       </c>
       <c r="H18" s="410" t="s">
-        <v>217</v>
+        <v>253</v>
       </c>
       <c r="I18" s="411">
         <v>5360</v>
@@ -25043,8 +25252,12 @@
         <f t="shared" si="1"/>
         <v>171520</v>
       </c>
-      <c r="O18" s="397"/>
-      <c r="P18" s="398"/>
+      <c r="O18" s="397" t="s">
+        <v>61</v>
+      </c>
+      <c r="P18" s="398">
+        <v>44645</v>
+      </c>
       <c r="Q18" s="66">
         <v>0</v>
       </c>
@@ -25055,7 +25268,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="92" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="U18" s="53"/>
       <c r="V18" s="54"/>
@@ -25078,7 +25291,9 @@
       <c r="G19" s="62">
         <v>44633</v>
       </c>
-      <c r="H19" s="410"/>
+      <c r="H19" s="410" t="s">
+        <v>242</v>
+      </c>
       <c r="I19" s="411">
         <v>21835</v>
       </c>
@@ -25097,13 +25312,17 @@
       </c>
       <c r="O19" s="397"/>
       <c r="P19" s="398"/>
-      <c r="Q19" s="79"/>
-      <c r="R19" s="67"/>
+      <c r="Q19" s="79">
+        <v>25140</v>
+      </c>
+      <c r="R19" s="67">
+        <v>44642</v>
+      </c>
       <c r="S19" s="51">
         <v>11200</v>
       </c>
       <c r="T19" s="92" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="U19" s="53"/>
       <c r="V19" s="54"/>
@@ -25112,7 +25331,7 @@
     </row>
     <row r="20" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="80" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B20" s="58" t="s">
         <v>32</v>
@@ -25126,7 +25345,9 @@
       <c r="G20" s="62">
         <v>44633</v>
       </c>
-      <c r="H20" s="410"/>
+      <c r="H20" s="410" t="s">
+        <v>242</v>
+      </c>
       <c r="I20" s="411">
         <v>5600</v>
       </c>
@@ -25145,13 +25366,17 @@
       </c>
       <c r="O20" s="89"/>
       <c r="P20" s="90"/>
-      <c r="Q20" s="79"/>
-      <c r="R20" s="67"/>
+      <c r="Q20" s="79">
+        <v>0</v>
+      </c>
+      <c r="R20" s="67">
+        <v>44642</v>
+      </c>
       <c r="S20" s="51">
         <v>0</v>
       </c>
       <c r="T20" s="92" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="U20" s="53"/>
       <c r="V20" s="54"/>
@@ -25159,116 +25384,196 @@
       <c r="X20" s="70"/>
     </row>
     <row r="21" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="78"/>
-      <c r="B21" s="58"/>
+      <c r="A21" s="78" t="s">
+        <v>224</v>
+      </c>
+      <c r="B21" s="58" t="s">
+        <v>31</v>
+      </c>
       <c r="C21" s="59"/>
       <c r="D21" s="60"/>
       <c r="E21" s="40"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="410"/>
-      <c r="I21" s="411"/>
+      <c r="F21" s="61">
+        <v>22290</v>
+      </c>
+      <c r="G21" s="62">
+        <v>44635</v>
+      </c>
+      <c r="H21" s="410" t="s">
+        <v>243</v>
+      </c>
+      <c r="I21" s="411">
+        <v>22920</v>
+      </c>
       <c r="J21" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="76"/>
+        <v>630</v>
+      </c>
+      <c r="K21" s="76">
+        <v>32.5</v>
+      </c>
       <c r="L21" s="65"/>
       <c r="M21" s="65"/>
       <c r="N21" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>744900</v>
       </c>
       <c r="O21" s="89"/>
       <c r="P21" s="90"/>
-      <c r="Q21" s="79"/>
-      <c r="R21" s="67"/>
-      <c r="S21" s="51"/>
-      <c r="T21" s="92"/>
+      <c r="Q21" s="79">
+        <v>25240</v>
+      </c>
+      <c r="R21" s="67">
+        <v>44642</v>
+      </c>
+      <c r="S21" s="51">
+        <v>11200</v>
+      </c>
+      <c r="T21" s="92" t="s">
+        <v>230</v>
+      </c>
       <c r="U21" s="53"/>
       <c r="V21" s="54"/>
       <c r="W21" s="53"/>
       <c r="X21" s="70"/>
     </row>
     <row r="22" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="81"/>
-      <c r="B22" s="58"/>
+      <c r="A22" s="81" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="58" t="s">
+        <v>37</v>
+      </c>
       <c r="C22" s="59"/>
       <c r="D22" s="60"/>
       <c r="E22" s="40"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="410"/>
-      <c r="I22" s="411"/>
+      <c r="F22" s="61">
+        <v>0</v>
+      </c>
+      <c r="G22" s="62">
+        <v>44635</v>
+      </c>
+      <c r="H22" s="410" t="s">
+        <v>243</v>
+      </c>
+      <c r="I22" s="411">
+        <v>5365</v>
+      </c>
       <c r="J22" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="76"/>
+        <v>5365</v>
+      </c>
+      <c r="K22" s="76">
+        <v>32.5</v>
+      </c>
       <c r="L22" s="65"/>
       <c r="M22" s="65"/>
       <c r="N22" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>174362.5</v>
       </c>
       <c r="O22" s="89"/>
       <c r="P22" s="90"/>
-      <c r="Q22" s="79"/>
-      <c r="R22" s="67"/>
-      <c r="S22" s="51"/>
-      <c r="T22" s="92"/>
+      <c r="Q22" s="79">
+        <v>0</v>
+      </c>
+      <c r="R22" s="67">
+        <v>44642</v>
+      </c>
+      <c r="S22" s="51">
+        <v>0</v>
+      </c>
+      <c r="T22" s="92" t="s">
+        <v>230</v>
+      </c>
       <c r="U22" s="53"/>
       <c r="V22" s="54"/>
       <c r="W22" s="53"/>
       <c r="X22" s="70"/>
     </row>
     <row r="23" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="82"/>
-      <c r="B23" s="58"/>
+      <c r="A23" s="82" t="s">
+        <v>225</v>
+      </c>
+      <c r="B23" s="58" t="s">
+        <v>72</v>
+      </c>
       <c r="C23" s="59"/>
       <c r="D23" s="60"/>
       <c r="E23" s="40"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="410"/>
-      <c r="I23" s="411"/>
+      <c r="F23" s="61">
+        <v>23040</v>
+      </c>
+      <c r="G23" s="62">
+        <v>44637</v>
+      </c>
+      <c r="H23" s="410" t="s">
+        <v>244</v>
+      </c>
+      <c r="I23" s="411">
+        <v>23330</v>
+      </c>
       <c r="J23" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="76"/>
+        <v>290</v>
+      </c>
+      <c r="K23" s="76">
+        <v>33</v>
+      </c>
       <c r="L23" s="65"/>
       <c r="M23" s="65"/>
       <c r="N23" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>769890</v>
       </c>
       <c r="O23" s="89"/>
       <c r="P23" s="90"/>
-      <c r="Q23" s="79"/>
-      <c r="R23" s="67"/>
-      <c r="S23" s="51"/>
-      <c r="T23" s="92"/>
+      <c r="Q23" s="79">
+        <v>25140</v>
+      </c>
+      <c r="R23" s="67">
+        <v>44642</v>
+      </c>
+      <c r="S23" s="51">
+        <v>11200</v>
+      </c>
+      <c r="T23" s="92" t="s">
+        <v>229</v>
+      </c>
       <c r="U23" s="53"/>
       <c r="V23" s="54"/>
       <c r="W23" s="53"/>
       <c r="X23" s="70"/>
     </row>
     <row r="24" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="83"/>
-      <c r="B24" s="58"/>
+      <c r="A24" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="58" t="s">
+        <v>37</v>
+      </c>
       <c r="C24" s="59"/>
       <c r="D24" s="60"/>
       <c r="E24" s="40"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="410"/>
-      <c r="I24" s="411"/>
+      <c r="F24" s="61">
+        <v>0</v>
+      </c>
+      <c r="G24" s="62">
+        <v>44637</v>
+      </c>
+      <c r="H24" s="410" t="s">
+        <v>244</v>
+      </c>
+      <c r="I24" s="411">
+        <v>0</v>
+      </c>
       <c r="J24" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K24" s="76"/>
+      <c r="K24" s="76">
+        <v>33</v>
+      </c>
       <c r="L24" s="65"/>
       <c r="M24" s="65"/>
       <c r="N24" s="48">
@@ -25277,74 +25582,126 @@
       </c>
       <c r="O24" s="397"/>
       <c r="P24" s="90"/>
-      <c r="Q24" s="79"/>
-      <c r="R24" s="67"/>
-      <c r="S24" s="91"/>
-      <c r="T24" s="92"/>
+      <c r="Q24" s="79">
+        <v>0</v>
+      </c>
+      <c r="R24" s="67">
+        <v>44642</v>
+      </c>
+      <c r="S24" s="91">
+        <v>0</v>
+      </c>
+      <c r="T24" s="92" t="s">
+        <v>229</v>
+      </c>
       <c r="U24" s="53"/>
       <c r="V24" s="54"/>
       <c r="W24" s="53"/>
       <c r="X24" s="70"/>
     </row>
     <row r="25" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="71"/>
-      <c r="B25" s="58"/>
+      <c r="A25" s="71" t="s">
+        <v>209</v>
+      </c>
+      <c r="B25" s="58" t="s">
+        <v>31</v>
+      </c>
       <c r="C25" s="59"/>
       <c r="D25" s="60"/>
       <c r="E25" s="40"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="410"/>
-      <c r="I25" s="411"/>
+      <c r="F25" s="61">
+        <v>21410</v>
+      </c>
+      <c r="G25" s="62">
+        <v>44638</v>
+      </c>
+      <c r="H25" s="410" t="s">
+        <v>245</v>
+      </c>
+      <c r="I25" s="411">
+        <v>21330</v>
+      </c>
       <c r="J25" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="76"/>
+        <v>-80</v>
+      </c>
+      <c r="K25" s="76">
+        <v>33</v>
+      </c>
       <c r="L25" s="65"/>
       <c r="M25" s="65"/>
       <c r="N25" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>703890</v>
       </c>
       <c r="O25" s="89"/>
       <c r="P25" s="90"/>
-      <c r="Q25" s="79"/>
-      <c r="R25" s="67"/>
-      <c r="S25" s="51"/>
-      <c r="T25" s="92"/>
+      <c r="Q25" s="79">
+        <v>25140</v>
+      </c>
+      <c r="R25" s="67">
+        <v>44642</v>
+      </c>
+      <c r="S25" s="51">
+        <v>11200</v>
+      </c>
+      <c r="T25" s="92" t="s">
+        <v>231</v>
+      </c>
       <c r="U25" s="53"/>
       <c r="V25" s="54"/>
       <c r="W25" s="53"/>
       <c r="X25" s="70"/>
     </row>
     <row r="26" spans="1:24" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="82"/>
-      <c r="B26" s="58"/>
+      <c r="A26" s="82" t="s">
+        <v>226</v>
+      </c>
+      <c r="B26" s="58" t="s">
+        <v>37</v>
+      </c>
       <c r="C26" s="59"/>
       <c r="D26" s="60"/>
       <c r="E26" s="40"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="410"/>
-      <c r="I26" s="411"/>
+      <c r="F26" s="61">
+        <v>0</v>
+      </c>
+      <c r="G26" s="62">
+        <v>44638</v>
+      </c>
+      <c r="H26" s="410" t="s">
+        <v>245</v>
+      </c>
+      <c r="I26" s="411">
+        <v>5375</v>
+      </c>
       <c r="J26" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K26" s="76"/>
+        <v>5375</v>
+      </c>
+      <c r="K26" s="76">
+        <v>33</v>
+      </c>
       <c r="L26" s="65"/>
       <c r="M26" s="65"/>
       <c r="N26" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>177375</v>
       </c>
       <c r="O26" s="89"/>
       <c r="P26" s="90"/>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="67"/>
-      <c r="S26" s="51"/>
-      <c r="T26" s="92"/>
+      <c r="Q26" s="79">
+        <v>0</v>
+      </c>
+      <c r="R26" s="67">
+        <v>44642</v>
+      </c>
+      <c r="S26" s="51">
+        <v>0</v>
+      </c>
+      <c r="T26" s="92" t="s">
+        <v>231</v>
+      </c>
       <c r="U26" s="53"/>
       <c r="V26" s="54"/>
       <c r="W26" s="53"/>
@@ -26273,33 +26630,49 @@
       <c r="U54" s="159"/>
       <c r="V54" s="160"/>
     </row>
-    <row r="55" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="80" t="s">
+    <row r="55" spans="1:24" s="161" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A55" s="499" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="438" t="s">
-        <v>23</v>
-      </c>
-      <c r="C55" s="439"/>
-      <c r="D55" s="440"/>
+        <v>24</v>
+      </c>
+      <c r="C55" s="464" t="s">
+        <v>232</v>
+      </c>
+      <c r="D55" s="439"/>
       <c r="E55" s="60"/>
-      <c r="F55" s="151"/>
-      <c r="G55" s="152"/>
-      <c r="H55" s="390"/>
-      <c r="I55" s="151"/>
+      <c r="F55" s="151">
+        <v>181.6</v>
+      </c>
+      <c r="G55" s="152">
+        <v>44627</v>
+      </c>
+      <c r="H55" s="502" t="s">
+        <v>233</v>
+      </c>
+      <c r="I55" s="151">
+        <v>181.6</v>
+      </c>
       <c r="J55" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K55" s="46"/>
+      <c r="K55" s="46">
+        <v>104</v>
+      </c>
       <c r="L55" s="65"/>
       <c r="M55" s="65"/>
       <c r="N55" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O55" s="89"/>
-      <c r="P55" s="162"/>
+        <v>18886.399999999998</v>
+      </c>
+      <c r="O55" s="460" t="s">
+        <v>59</v>
+      </c>
+      <c r="P55" s="454">
+        <v>44645</v>
+      </c>
       <c r="Q55" s="128"/>
       <c r="R55" s="158"/>
       <c r="S55" s="92"/>
@@ -26308,30 +26681,38 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="80"/>
+      <c r="A56" s="501"/>
       <c r="B56" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="439"/>
-      <c r="D56" s="441"/>
+      <c r="C56" s="465"/>
+      <c r="D56" s="440"/>
       <c r="E56" s="60"/>
-      <c r="F56" s="151"/>
-      <c r="G56" s="152"/>
-      <c r="H56" s="390"/>
-      <c r="I56" s="151"/>
+      <c r="F56" s="151">
+        <v>967</v>
+      </c>
+      <c r="G56" s="152">
+        <v>44627</v>
+      </c>
+      <c r="H56" s="503"/>
+      <c r="I56" s="151">
+        <v>967</v>
+      </c>
       <c r="J56" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K56" s="46"/>
+      <c r="K56" s="46">
+        <v>96</v>
+      </c>
       <c r="L56" s="65"/>
       <c r="M56" s="65"/>
       <c r="N56" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O56" s="164"/>
-      <c r="P56" s="162"/>
+        <v>92832</v>
+      </c>
+      <c r="O56" s="461"/>
+      <c r="P56" s="455"/>
       <c r="Q56" s="164"/>
       <c r="R56" s="158"/>
       <c r="S56" s="92"/>
@@ -26346,7 +26727,7 @@
       <c r="B57" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="442"/>
+      <c r="C57" s="441"/>
       <c r="D57" s="168"/>
       <c r="E57" s="60"/>
       <c r="F57" s="151"/>
@@ -26378,7 +26759,7 @@
       <c r="B58" s="438" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="442"/>
+      <c r="C58" s="441"/>
       <c r="D58" s="168"/>
       <c r="E58" s="60"/>
       <c r="F58" s="151"/>
@@ -26410,8 +26791,8 @@
       <c r="B59" s="438" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="443"/>
-      <c r="D59" s="441"/>
+      <c r="C59" s="442"/>
+      <c r="D59" s="440"/>
       <c r="E59" s="60"/>
       <c r="F59" s="151"/>
       <c r="G59" s="152"/>
@@ -26444,7 +26825,7 @@
       <c r="B60" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="443"/>
+      <c r="C60" s="442"/>
       <c r="D60" s="168"/>
       <c r="E60" s="60"/>
       <c r="F60" s="151"/>
@@ -26502,30 +26883,48 @@
       <c r="V61" s="54"/>
     </row>
     <row r="62" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A62" s="82"/>
+      <c r="A62" s="504" t="s">
+        <v>106</v>
+      </c>
       <c r="B62" s="178" t="s">
-        <v>155</v>
-      </c>
-      <c r="C62" s="171"/>
+        <v>246</v>
+      </c>
+      <c r="C62" s="506" t="s">
+        <v>247</v>
+      </c>
       <c r="D62" s="168"/>
       <c r="E62" s="60"/>
-      <c r="F62" s="151"/>
-      <c r="G62" s="152"/>
-      <c r="H62" s="153"/>
-      <c r="I62" s="151"/>
+      <c r="F62" s="151">
+        <v>152.6</v>
+      </c>
+      <c r="G62" s="152">
+        <v>44622</v>
+      </c>
+      <c r="H62" s="508">
+        <v>37162</v>
+      </c>
+      <c r="I62" s="151">
+        <v>152.6</v>
+      </c>
       <c r="J62" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K62" s="166"/>
+      <c r="K62" s="166">
+        <v>51</v>
+      </c>
       <c r="L62" s="99"/>
       <c r="M62" s="99"/>
       <c r="N62" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O62" s="164"/>
-      <c r="P62" s="162"/>
+        <v>7782.5999999999995</v>
+      </c>
+      <c r="O62" s="460" t="s">
+        <v>61</v>
+      </c>
+      <c r="P62" s="454">
+        <v>44643</v>
+      </c>
       <c r="Q62" s="164"/>
       <c r="R62" s="129"/>
       <c r="S62" s="92"/>
@@ -26534,30 +26933,38 @@
       <c r="V62" s="54"/>
     </row>
     <row r="63" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="82"/>
+      <c r="A63" s="505"/>
       <c r="B63" s="178" t="s">
-        <v>157</v>
-      </c>
-      <c r="C63" s="171"/>
+        <v>248</v>
+      </c>
+      <c r="C63" s="507"/>
       <c r="D63" s="168"/>
       <c r="E63" s="60"/>
-      <c r="F63" s="151"/>
-      <c r="G63" s="152"/>
-      <c r="H63" s="153"/>
-      <c r="I63" s="151"/>
+      <c r="F63" s="151">
+        <v>204.8</v>
+      </c>
+      <c r="G63" s="152">
+        <v>44622</v>
+      </c>
+      <c r="H63" s="509"/>
+      <c r="I63" s="151">
+        <v>204.8</v>
+      </c>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K63" s="166"/>
+      <c r="K63" s="166">
+        <v>83</v>
+      </c>
       <c r="L63" s="99"/>
       <c r="M63" s="99"/>
       <c r="N63" s="48">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O63" s="164"/>
-      <c r="P63" s="162"/>
+        <v>16998.400000000001</v>
+      </c>
+      <c r="O63" s="461"/>
+      <c r="P63" s="455"/>
       <c r="Q63" s="164"/>
       <c r="R63" s="129"/>
       <c r="S63" s="92"/>
@@ -26567,9 +26974,7 @@
     </row>
     <row r="64" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="80"/>
-      <c r="B64" s="178" t="s">
-        <v>153</v>
-      </c>
+      <c r="B64" s="178"/>
       <c r="C64" s="183"/>
       <c r="D64" s="171"/>
       <c r="E64" s="60"/>
@@ -27038,8 +27443,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="475"/>
-      <c r="P79" s="477"/>
+      <c r="O79" s="460"/>
+      <c r="P79" s="474"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -27068,8 +27473,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="476"/>
-      <c r="P80" s="478"/>
+      <c r="O80" s="461"/>
+      <c r="P80" s="475"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -27098,8 +27503,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="475"/>
-      <c r="P81" s="477"/>
+      <c r="O81" s="460"/>
+      <c r="P81" s="474"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -27131,8 +27536,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="476"/>
-      <c r="P82" s="478"/>
+      <c r="O82" s="461"/>
+      <c r="P82" s="475"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -27290,8 +27695,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="479"/>
-      <c r="M87" s="480"/>
+      <c r="L87" s="476"/>
+      <c r="M87" s="477"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -27323,8 +27728,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="479"/>
-      <c r="M88" s="480"/>
+      <c r="L88" s="476"/>
+      <c r="M88" s="477"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -27527,8 +27932,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="475"/>
-      <c r="P94" s="471"/>
+      <c r="O94" s="460"/>
+      <c r="P94" s="470"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -27560,8 +27965,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="476"/>
-      <c r="P95" s="472"/>
+      <c r="O95" s="461"/>
+      <c r="P95" s="471"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -32953,14 +33358,14 @@
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="473" t="s">
+      <c r="F259" s="472" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="473"/>
-      <c r="H259" s="474"/>
+      <c r="G259" s="472"/>
+      <c r="H259" s="473"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
-        <v>236185</v>
+        <v>316010.99999999994</v>
       </c>
       <c r="J259" s="318"/>
       <c r="K259" s="314"/>
@@ -33059,17 +33464,17 @@
       <c r="M263" s="336"/>
       <c r="N263" s="337">
         <f>SUM(N4:N262)</f>
-        <v>14506081.5</v>
+        <v>10440498.4</v>
       </c>
       <c r="O263" s="338"/>
       <c r="Q263" s="339">
         <f>SUM(Q4:Q262)</f>
-        <v>174200</v>
+        <v>274860</v>
       </c>
       <c r="R263" s="8"/>
       <c r="S263" s="340">
         <f>SUM(S17:S262)</f>
-        <v>22400</v>
+        <v>56000</v>
       </c>
       <c r="T263" s="341"/>
       <c r="U263" s="342"/>
@@ -33119,7 +33524,7 @@
       <c r="M266" s="352"/>
       <c r="N266" s="353">
         <f>V263+S263+Q263+N263+L263</f>
-        <v>14702681.5</v>
+        <v>10771358.4</v>
       </c>
       <c r="O266" s="354"/>
       <c r="R266" s="324"/>
@@ -33530,7 +33935,22 @@
       <c r="V292"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="22">
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="S1:T2"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="O55:O56"/>
+    <mergeCell ref="P55:P56"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="O62:O63"/>
+    <mergeCell ref="P62:P63"/>
     <mergeCell ref="O94:O95"/>
     <mergeCell ref="P94:P95"/>
     <mergeCell ref="F259:H259"/>
@@ -33538,11 +33958,6 @@
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="O81:O82"/>
     <mergeCell ref="P81:P82"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="S1:T2"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="L87:M88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRE 7 ABR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #03  MARZO  2022/ENTRADAS OBRADOR  MaRzO     2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #03  MARZO  2022/ENTRADAS OBRADOR  MaRzO     2022.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="299">
   <si>
     <t>FECHA DE PAGO</t>
   </si>
@@ -891,6 +891,39 @@
   </si>
   <si>
     <t>0322 Z</t>
+  </si>
+  <si>
+    <t>0330 Z</t>
+  </si>
+  <si>
+    <t>0341 Z</t>
+  </si>
+  <si>
+    <t>0357 Z</t>
+  </si>
+  <si>
+    <t>0369 Z</t>
+  </si>
+  <si>
+    <t>0388 Z</t>
+  </si>
+  <si>
+    <t>0393 Z</t>
+  </si>
+  <si>
+    <t>0402 Z</t>
+  </si>
+  <si>
+    <t>0417 Z</t>
+  </si>
+  <si>
+    <t>0432 Z</t>
+  </si>
+  <si>
+    <t>0442 Z</t>
+  </si>
+  <si>
+    <t>0453 Z</t>
   </si>
 </sst>
 </file>
@@ -2218,7 +2251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="518">
+  <cellXfs count="519">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3463,6 +3496,102 @@
     <xf numFmtId="0" fontId="22" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3480,99 +3609,6 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="11" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="11" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3959,18 +3995,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="486" t="s">
+      <c r="A1" s="463" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="486"/>
-      <c r="C1" s="486"/>
-      <c r="D1" s="486"/>
-      <c r="E1" s="486"/>
-      <c r="F1" s="486"/>
-      <c r="G1" s="486"/>
-      <c r="H1" s="486"/>
-      <c r="I1" s="486"/>
-      <c r="J1" s="486"/>
+      <c r="B1" s="463"/>
+      <c r="C1" s="463"/>
+      <c r="D1" s="463"/>
+      <c r="E1" s="463"/>
+      <c r="F1" s="463"/>
+      <c r="G1" s="463"/>
+      <c r="H1" s="463"/>
+      <c r="I1" s="463"/>
+      <c r="J1" s="463"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
@@ -3984,22 +4020,22 @@
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="487" t="s">
+      <c r="W1" s="464" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="488"/>
+      <c r="X1" s="465"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="486"/>
-      <c r="B2" s="486"/>
-      <c r="C2" s="486"/>
-      <c r="D2" s="486"/>
-      <c r="E2" s="486"/>
-      <c r="F2" s="486"/>
-      <c r="G2" s="486"/>
-      <c r="H2" s="486"/>
-      <c r="I2" s="486"/>
-      <c r="J2" s="486"/>
+      <c r="A2" s="463"/>
+      <c r="B2" s="463"/>
+      <c r="C2" s="463"/>
+      <c r="D2" s="463"/>
+      <c r="E2" s="463"/>
+      <c r="F2" s="463"/>
+      <c r="G2" s="463"/>
+      <c r="H2" s="463"/>
+      <c r="I2" s="463"/>
+      <c r="J2" s="463"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -4053,10 +4089,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="489" t="s">
+      <c r="O3" s="466" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="490"/>
+      <c r="P3" s="467"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -4600,7 +4636,7 @@
       <c r="B12" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="491" t="s">
+      <c r="C12" s="468" t="s">
         <v>103</v>
       </c>
       <c r="D12" s="400"/>
@@ -4664,7 +4700,7 @@
       <c r="B13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="492"/>
+      <c r="C13" s="469"/>
       <c r="D13" s="400"/>
       <c r="E13" s="401"/>
       <c r="F13" s="402">
@@ -6666,13 +6702,13 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="470" t="s">
+      <c r="A56" s="480" t="s">
         <v>41</v>
       </c>
       <c r="B56" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="472" t="s">
+      <c r="C56" s="482" t="s">
         <v>110</v>
       </c>
       <c r="D56" s="150"/>
@@ -6712,11 +6748,11 @@
       <c r="V56" s="160"/>
     </row>
     <row r="57" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="471"/>
+      <c r="A57" s="481"/>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="473"/>
+      <c r="C57" s="483"/>
       <c r="D57" s="150"/>
       <c r="E57" s="40"/>
       <c r="F57" s="151">
@@ -6752,13 +6788,13 @@
       <c r="V57" s="160"/>
     </row>
     <row r="58" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="470" t="s">
+      <c r="A58" s="480" t="s">
         <v>41</v>
       </c>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="472" t="s">
+      <c r="C58" s="482" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="150"/>
@@ -6791,7 +6827,7 @@
       <c r="O58" s="476" t="s">
         <v>59</v>
       </c>
-      <c r="P58" s="497">
+      <c r="P58" s="478">
         <v>44606</v>
       </c>
       <c r="Q58" s="128"/>
@@ -6802,11 +6838,11 @@
       <c r="V58" s="160"/>
     </row>
     <row r="59" spans="1:24" s="161" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="471"/>
+      <c r="A59" s="481"/>
       <c r="B59" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="473"/>
+      <c r="C59" s="483"/>
       <c r="D59" s="150"/>
       <c r="E59" s="40"/>
       <c r="F59" s="151">
@@ -6833,7 +6869,7 @@
         <v>22440</v>
       </c>
       <c r="O59" s="477"/>
-      <c r="P59" s="498"/>
+      <c r="P59" s="479"/>
       <c r="Q59" s="128"/>
       <c r="R59" s="158"/>
       <c r="S59" s="92"/>
@@ -6842,13 +6878,13 @@
       <c r="V59" s="160"/>
     </row>
     <row r="60" spans="1:24" s="161" customFormat="1" ht="48.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="495" t="s">
+      <c r="A60" s="472" t="s">
         <v>41</v>
       </c>
       <c r="B60" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="493" t="s">
+      <c r="C60" s="470" t="s">
         <v>109</v>
       </c>
       <c r="D60" s="163"/>
@@ -6884,7 +6920,7 @@
       <c r="O60" s="476" t="s">
         <v>59</v>
       </c>
-      <c r="P60" s="497">
+      <c r="P60" s="478">
         <v>44594</v>
       </c>
       <c r="Q60" s="164"/>
@@ -6897,11 +6933,11 @@
       <c r="X60"/>
     </row>
     <row r="61" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="496"/>
+      <c r="A61" s="473"/>
       <c r="B61" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="494"/>
+      <c r="C61" s="471"/>
       <c r="D61" s="165"/>
       <c r="E61" s="40">
         <f t="shared" si="2"/>
@@ -6931,7 +6967,7 @@
         <v>23623.200000000001</v>
       </c>
       <c r="O61" s="477"/>
-      <c r="P61" s="498"/>
+      <c r="P61" s="479"/>
       <c r="Q61" s="164"/>
       <c r="R61" s="129"/>
       <c r="S61" s="92"/>
@@ -6997,7 +7033,7 @@
       <c r="B63" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="464"/>
+      <c r="C63" s="496"/>
       <c r="D63" s="163"/>
       <c r="E63" s="40">
         <f t="shared" si="2"/>
@@ -7005,7 +7041,7 @@
       </c>
       <c r="F63" s="151"/>
       <c r="G63" s="152"/>
-      <c r="H63" s="466"/>
+      <c r="H63" s="498"/>
       <c r="I63" s="151"/>
       <c r="J63" s="45">
         <f t="shared" si="0"/>
@@ -7034,7 +7070,7 @@
       <c r="B64" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="465"/>
+      <c r="C64" s="497"/>
       <c r="D64" s="168"/>
       <c r="E64" s="40">
         <f t="shared" si="2"/>
@@ -7042,7 +7078,7 @@
       </c>
       <c r="F64" s="151"/>
       <c r="G64" s="152"/>
-      <c r="H64" s="467"/>
+      <c r="H64" s="499"/>
       <c r="I64" s="151"/>
       <c r="J64" s="45">
         <f t="shared" si="0"/>
@@ -7220,8 +7256,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O68" s="468"/>
-      <c r="P68" s="462"/>
+      <c r="O68" s="488"/>
+      <c r="P68" s="494"/>
       <c r="Q68" s="164"/>
       <c r="R68" s="129"/>
       <c r="S68" s="180"/>
@@ -7255,8 +7291,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O69" s="469"/>
-      <c r="P69" s="463"/>
+      <c r="O69" s="489"/>
+      <c r="P69" s="495"/>
       <c r="Q69" s="164"/>
       <c r="R69" s="129"/>
       <c r="S69" s="180"/>
@@ -7746,8 +7782,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="468"/>
-      <c r="P82" s="482"/>
+      <c r="O82" s="488"/>
+      <c r="P82" s="490"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="129"/>
       <c r="S82" s="180"/>
@@ -7779,8 +7815,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O83" s="469"/>
-      <c r="P83" s="483"/>
+      <c r="O83" s="489"/>
+      <c r="P83" s="491"/>
       <c r="Q83" s="164"/>
       <c r="R83" s="129"/>
       <c r="S83" s="180"/>
@@ -7812,8 +7848,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O84" s="468"/>
-      <c r="P84" s="482"/>
+      <c r="O84" s="488"/>
+      <c r="P84" s="490"/>
       <c r="Q84" s="164"/>
       <c r="R84" s="158"/>
       <c r="S84" s="180"/>
@@ -7845,8 +7881,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O85" s="469"/>
-      <c r="P85" s="483"/>
+      <c r="O85" s="489"/>
+      <c r="P85" s="491"/>
       <c r="Q85" s="164"/>
       <c r="R85" s="158"/>
       <c r="S85" s="180"/>
@@ -8004,8 +8040,8 @@
         <v>0</v>
       </c>
       <c r="K90" s="100"/>
-      <c r="L90" s="484"/>
-      <c r="M90" s="485"/>
+      <c r="L90" s="492"/>
+      <c r="M90" s="493"/>
       <c r="N90" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8037,8 +8073,8 @@
         <v>0</v>
       </c>
       <c r="K91" s="100"/>
-      <c r="L91" s="484"/>
-      <c r="M91" s="485"/>
+      <c r="L91" s="492"/>
+      <c r="M91" s="493"/>
       <c r="N91" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -8241,8 +8277,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O97" s="468"/>
-      <c r="P97" s="478"/>
+      <c r="O97" s="488"/>
+      <c r="P97" s="484"/>
       <c r="Q97" s="164"/>
       <c r="R97" s="129"/>
       <c r="S97" s="180"/>
@@ -8274,8 +8310,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O98" s="469"/>
-      <c r="P98" s="479"/>
+      <c r="O98" s="489"/>
+      <c r="P98" s="485"/>
       <c r="Q98" s="164"/>
       <c r="R98" s="129"/>
       <c r="S98" s="180"/>
@@ -13667,11 +13703,11 @@
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F262" s="480" t="s">
+      <c r="F262" s="486" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="480"/>
-      <c r="H262" s="481"/>
+      <c r="G262" s="486"/>
+      <c r="H262" s="487"/>
       <c r="I262" s="317">
         <f>SUM(I4:I261)</f>
         <v>426245.47000000003</v>
@@ -14245,6 +14281,22 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="P68:P69"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="H63:H64"/>
+    <mergeCell ref="O68:O69"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="O58:O59"/>
+    <mergeCell ref="P97:P98"/>
+    <mergeCell ref="F262:H262"/>
+    <mergeCell ref="O82:O83"/>
+    <mergeCell ref="P82:P83"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="P84:P85"/>
+    <mergeCell ref="L90:M91"/>
+    <mergeCell ref="O97:O98"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="O3:P3"/>
@@ -14258,22 +14310,6 @@
     <mergeCell ref="C56:C57"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="P58:P59"/>
-    <mergeCell ref="P97:P98"/>
-    <mergeCell ref="F262:H262"/>
-    <mergeCell ref="O82:O83"/>
-    <mergeCell ref="P82:P83"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="P84:P85"/>
-    <mergeCell ref="L90:M91"/>
-    <mergeCell ref="O97:O98"/>
-    <mergeCell ref="P68:P69"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="O68:O69"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="O58:O59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -14320,49 +14356,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="486" t="s">
+      <c r="A1" s="463" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="486"/>
-      <c r="C1" s="486"/>
-      <c r="D1" s="486"/>
-      <c r="E1" s="486"/>
-      <c r="F1" s="486"/>
-      <c r="G1" s="486"/>
-      <c r="H1" s="486"/>
-      <c r="I1" s="486"/>
-      <c r="J1" s="486"/>
+      <c r="B1" s="463"/>
+      <c r="C1" s="463"/>
+      <c r="D1" s="463"/>
+      <c r="E1" s="463"/>
+      <c r="F1" s="463"/>
+      <c r="G1" s="463"/>
+      <c r="H1" s="463"/>
+      <c r="I1" s="463"/>
+      <c r="J1" s="463"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="505" t="s">
+      <c r="S1" s="506" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="505"/>
+      <c r="T1" s="506"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="487" t="s">
+      <c r="W1" s="464" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="488"/>
+      <c r="X1" s="465"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="486"/>
-      <c r="B2" s="486"/>
-      <c r="C2" s="486"/>
-      <c r="D2" s="486"/>
-      <c r="E2" s="486"/>
-      <c r="F2" s="486"/>
-      <c r="G2" s="486"/>
-      <c r="H2" s="486"/>
-      <c r="I2" s="486"/>
-      <c r="J2" s="486"/>
+      <c r="A2" s="463"/>
+      <c r="B2" s="463"/>
+      <c r="C2" s="463"/>
+      <c r="D2" s="463"/>
+      <c r="E2" s="463"/>
+      <c r="F2" s="463"/>
+      <c r="G2" s="463"/>
+      <c r="H2" s="463"/>
+      <c r="I2" s="463"/>
+      <c r="J2" s="463"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -14370,8 +14406,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="506"/>
-      <c r="T2" s="506"/>
+      <c r="S2" s="507"/>
+      <c r="T2" s="507"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -14416,10 +14452,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="489" t="s">
+      <c r="O3" s="466" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="490"/>
+      <c r="P3" s="467"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -17055,13 +17091,13 @@
       <c r="V54" s="160"/>
     </row>
     <row r="55" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="507" t="s">
+      <c r="A55" s="508" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="472" t="s">
+      <c r="C55" s="482" t="s">
         <v>160</v>
       </c>
       <c r="D55" s="150"/>
@@ -17072,7 +17108,7 @@
       <c r="G55" s="152">
         <v>44599</v>
       </c>
-      <c r="H55" s="466" t="s">
+      <c r="H55" s="498" t="s">
         <v>161</v>
       </c>
       <c r="I55" s="151">
@@ -17101,11 +17137,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="508"/>
+      <c r="A56" s="509"/>
       <c r="B56" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="473"/>
+      <c r="C56" s="483"/>
       <c r="D56" s="163"/>
       <c r="E56" s="40"/>
       <c r="F56" s="151">
@@ -17114,7 +17150,7 @@
       <c r="G56" s="152">
         <v>44599</v>
       </c>
-      <c r="H56" s="467"/>
+      <c r="H56" s="499"/>
       <c r="I56" s="151">
         <v>194.4</v>
       </c>
@@ -17143,13 +17179,13 @@
       <c r="X56"/>
     </row>
     <row r="57" spans="1:24" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="499" t="s">
+      <c r="A57" s="500" t="s">
         <v>41</v>
       </c>
       <c r="B57" s="148" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="501" t="s">
+      <c r="C57" s="502" t="s">
         <v>162</v>
       </c>
       <c r="D57" s="165"/>
@@ -17160,7 +17196,7 @@
       <c r="G57" s="152">
         <v>44606</v>
       </c>
-      <c r="H57" s="466" t="s">
+      <c r="H57" s="498" t="s">
         <v>163</v>
       </c>
       <c r="I57" s="151">
@@ -17179,10 +17215,10 @@
         <f t="shared" si="1"/>
         <v>35776</v>
       </c>
-      <c r="O57" s="468" t="s">
+      <c r="O57" s="488" t="s">
         <v>59</v>
       </c>
-      <c r="P57" s="462">
+      <c r="P57" s="494">
         <v>44620</v>
       </c>
       <c r="Q57" s="164"/>
@@ -17193,11 +17229,11 @@
       <c r="V57" s="54"/>
     </row>
     <row r="58" spans="1:24" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="500"/>
+      <c r="A58" s="501"/>
       <c r="B58" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="502"/>
+      <c r="C58" s="503"/>
       <c r="D58" s="165"/>
       <c r="E58" s="40"/>
       <c r="F58" s="151">
@@ -17206,7 +17242,7 @@
       <c r="G58" s="152">
         <v>44606</v>
       </c>
-      <c r="H58" s="467"/>
+      <c r="H58" s="499"/>
       <c r="I58" s="151">
         <v>627.60209999999995</v>
       </c>
@@ -17223,8 +17259,8 @@
         <f t="shared" si="1"/>
         <v>58366.995299999995</v>
       </c>
-      <c r="O58" s="503"/>
-      <c r="P58" s="504"/>
+      <c r="O58" s="504"/>
+      <c r="P58" s="505"/>
       <c r="Q58" s="164"/>
       <c r="R58" s="129"/>
       <c r="S58" s="92"/>
@@ -17232,7 +17268,7 @@
       <c r="U58" s="53"/>
       <c r="V58" s="54"/>
     </row>
-    <row r="59" spans="1:24" s="161" customFormat="1" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:24" s="161" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="449" t="s">
         <v>41</v>
       </c>
@@ -17250,7 +17286,7 @@
       <c r="G59" s="152">
         <v>44613</v>
       </c>
-      <c r="H59" s="466" t="s">
+      <c r="H59" s="498" t="s">
         <v>228</v>
       </c>
       <c r="I59" s="151">
@@ -17294,7 +17330,7 @@
       <c r="E60" s="40"/>
       <c r="F60" s="151"/>
       <c r="G60" s="152"/>
-      <c r="H60" s="467"/>
+      <c r="H60" s="499"/>
       <c r="I60" s="151"/>
       <c r="J60" s="45">
         <f t="shared" si="0"/>
@@ -17957,8 +17993,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="468"/>
-      <c r="P79" s="482"/>
+      <c r="O79" s="488"/>
+      <c r="P79" s="490"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -17987,8 +18023,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="469"/>
-      <c r="P80" s="483"/>
+      <c r="O80" s="489"/>
+      <c r="P80" s="491"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -18017,8 +18053,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="468"/>
-      <c r="P81" s="482"/>
+      <c r="O81" s="488"/>
+      <c r="P81" s="490"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -18050,8 +18086,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="469"/>
-      <c r="P82" s="483"/>
+      <c r="O82" s="489"/>
+      <c r="P82" s="491"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -18209,8 +18245,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="484"/>
-      <c r="M87" s="485"/>
+      <c r="L87" s="492"/>
+      <c r="M87" s="493"/>
       <c r="N87" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -18242,8 +18278,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="484"/>
-      <c r="M88" s="485"/>
+      <c r="L88" s="492"/>
+      <c r="M88" s="493"/>
       <c r="N88" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -18446,8 +18482,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="468"/>
-      <c r="P94" s="478"/>
+      <c r="O94" s="488"/>
+      <c r="P94" s="484"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -18479,8 +18515,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="469"/>
-      <c r="P95" s="479"/>
+      <c r="O95" s="489"/>
+      <c r="P95" s="485"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -23872,11 +23908,11 @@
         <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="480" t="s">
+      <c r="F259" s="486" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="480"/>
-      <c r="H259" s="481"/>
+      <c r="G259" s="486"/>
+      <c r="H259" s="487"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>387207.97210000001</v>
@@ -24450,12 +24486,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="L87:M88"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
     <mergeCell ref="O79:O80"/>
     <mergeCell ref="P79:P80"/>
     <mergeCell ref="A1:J2"/>
@@ -24471,6 +24501,12 @@
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="H55:H56"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="L87:M88"/>
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -24485,10 +24521,10 @@
   <dimension ref="A1:X292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="R4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="R22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -24517,49 +24553,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="486" t="s">
+      <c r="A1" s="463" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="486"/>
-      <c r="C1" s="486"/>
-      <c r="D1" s="486"/>
-      <c r="E1" s="486"/>
-      <c r="F1" s="486"/>
-      <c r="G1" s="486"/>
-      <c r="H1" s="486"/>
-      <c r="I1" s="486"/>
-      <c r="J1" s="486"/>
+      <c r="B1" s="463"/>
+      <c r="C1" s="463"/>
+      <c r="D1" s="463"/>
+      <c r="E1" s="463"/>
+      <c r="F1" s="463"/>
+      <c r="G1" s="463"/>
+      <c r="H1" s="463"/>
+      <c r="I1" s="463"/>
+      <c r="J1" s="463"/>
       <c r="K1" s="375"/>
       <c r="L1" s="375"/>
       <c r="M1" s="375"/>
       <c r="N1" s="375"/>
       <c r="O1" s="376"/>
-      <c r="S1" s="505" t="s">
+      <c r="S1" s="506" t="s">
         <v>142</v>
       </c>
-      <c r="T1" s="505"/>
+      <c r="T1" s="506"/>
       <c r="U1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="487" t="s">
+      <c r="W1" s="464" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="488"/>
+      <c r="X1" s="465"/>
     </row>
     <row r="2" spans="1:24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="486"/>
-      <c r="B2" s="486"/>
-      <c r="C2" s="486"/>
-      <c r="D2" s="486"/>
-      <c r="E2" s="486"/>
-      <c r="F2" s="486"/>
-      <c r="G2" s="486"/>
-      <c r="H2" s="486"/>
-      <c r="I2" s="486"/>
-      <c r="J2" s="486"/>
+      <c r="A2" s="463"/>
+      <c r="B2" s="463"/>
+      <c r="C2" s="463"/>
+      <c r="D2" s="463"/>
+      <c r="E2" s="463"/>
+      <c r="F2" s="463"/>
+      <c r="G2" s="463"/>
+      <c r="H2" s="463"/>
+      <c r="I2" s="463"/>
+      <c r="J2" s="463"/>
       <c r="K2" s="377"/>
       <c r="L2" s="377"/>
       <c r="M2" s="377"/>
@@ -24567,8 +24603,8 @@
       <c r="O2" s="379"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11"/>
-      <c r="S2" s="506"/>
-      <c r="T2" s="506"/>
+      <c r="S2" s="507"/>
+      <c r="T2" s="507"/>
       <c r="U2" s="14"/>
       <c r="V2" s="15"/>
       <c r="W2" s="16"/>
@@ -24613,10 +24649,10 @@
       <c r="N3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="489" t="s">
+      <c r="O3" s="466" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="490"/>
+      <c r="P3" s="467"/>
       <c r="Q3" s="30" t="s">
         <v>16</v>
       </c>
@@ -24783,11 +24819,15 @@
       <c r="B6" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60"/>
+      <c r="C6" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="D6" s="60">
+        <v>46</v>
+      </c>
       <c r="E6" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1010620</v>
       </c>
       <c r="F6" s="61">
         <v>21970</v>
@@ -24848,8 +24888,12 @@
       <c r="B7" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="60"/>
+      <c r="C7" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="D7" s="60">
+        <v>0</v>
+      </c>
       <c r="E7" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -24913,11 +24957,15 @@
       <c r="B8" s="58" t="s">
         <v>191</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="60"/>
+      <c r="C8" s="59" t="s">
+        <v>289</v>
+      </c>
+      <c r="D8" s="60">
+        <v>46</v>
+      </c>
       <c r="E8" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>976120</v>
       </c>
       <c r="F8" s="61">
         <v>21220</v>
@@ -24978,8 +25026,12 @@
       <c r="B9" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="60"/>
+      <c r="C9" s="59" t="s">
+        <v>289</v>
+      </c>
+      <c r="D9" s="60">
+        <v>0</v>
+      </c>
       <c r="E9" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -25043,11 +25095,15 @@
       <c r="B10" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="72"/>
+      <c r="C10" s="59" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" s="72">
+        <v>39</v>
+      </c>
       <c r="E10" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>858390</v>
       </c>
       <c r="F10" s="61">
         <v>22010</v>
@@ -25108,8 +25164,12 @@
       <c r="B11" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="59"/>
-      <c r="D11" s="60"/>
+      <c r="C11" s="59" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11" s="60">
+        <v>0</v>
+      </c>
       <c r="E11" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -25173,9 +25233,11 @@
       <c r="B12" s="58" t="s">
         <v>205</v>
       </c>
-      <c r="C12" s="431"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="40">
+      <c r="C12" s="462"/>
+      <c r="D12" s="87">
+        <v>0</v>
+      </c>
+      <c r="E12" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -25238,11 +25300,15 @@
       <c r="B13" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="432"/>
-      <c r="D13" s="60"/>
+      <c r="C13" s="432" t="s">
+        <v>291</v>
+      </c>
+      <c r="D13" s="60">
+        <v>46</v>
+      </c>
       <c r="E13" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1037300</v>
       </c>
       <c r="F13" s="61">
         <v>22550</v>
@@ -25303,8 +25369,12 @@
       <c r="B14" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="59"/>
-      <c r="D14" s="60"/>
+      <c r="C14" s="59" t="s">
+        <v>291</v>
+      </c>
+      <c r="D14" s="60">
+        <v>0</v>
+      </c>
       <c r="E14" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -25368,11 +25438,15 @@
       <c r="B15" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60"/>
+      <c r="C15" s="59" t="s">
+        <v>292</v>
+      </c>
+      <c r="D15" s="60">
+        <v>46</v>
+      </c>
       <c r="E15" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>941160</v>
       </c>
       <c r="F15" s="61">
         <v>20460</v>
@@ -25433,8 +25507,12 @@
       <c r="B16" s="58" t="s">
         <v>208</v>
       </c>
-      <c r="C16" s="74"/>
-      <c r="D16" s="60"/>
+      <c r="C16" s="74" t="s">
+        <v>292</v>
+      </c>
+      <c r="D16" s="60">
+        <v>0</v>
+      </c>
       <c r="E16" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -25498,11 +25576,15 @@
       <c r="B17" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="60"/>
+      <c r="C17" s="59" t="s">
+        <v>293</v>
+      </c>
+      <c r="D17" s="60">
+        <v>46</v>
+      </c>
       <c r="E17" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1080540</v>
       </c>
       <c r="F17" s="61">
         <v>23490</v>
@@ -25563,8 +25645,12 @@
       <c r="B18" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="60"/>
+      <c r="C18" s="59" t="s">
+        <v>293</v>
+      </c>
+      <c r="D18" s="60">
+        <v>0</v>
+      </c>
       <c r="E18" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -25628,11 +25714,15 @@
       <c r="B19" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="60"/>
+      <c r="C19" s="59" t="s">
+        <v>294</v>
+      </c>
+      <c r="D19" s="60">
+        <v>46</v>
+      </c>
       <c r="E19" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>994980</v>
       </c>
       <c r="F19" s="61">
         <v>21630</v>
@@ -25693,8 +25783,12 @@
       <c r="B20" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="60"/>
+      <c r="C20" s="59" t="s">
+        <v>294</v>
+      </c>
+      <c r="D20" s="60">
+        <v>0</v>
+      </c>
       <c r="E20" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -25758,11 +25852,15 @@
       <c r="B21" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="59"/>
-      <c r="D21" s="60"/>
+      <c r="C21" s="59" t="s">
+        <v>295</v>
+      </c>
+      <c r="D21" s="60">
+        <v>46</v>
+      </c>
       <c r="E21" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1025340</v>
       </c>
       <c r="F21" s="61">
         <v>22290</v>
@@ -25823,8 +25921,12 @@
       <c r="B22" s="58" t="s">
         <v>265</v>
       </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="60"/>
+      <c r="C22" s="59" t="s">
+        <v>295</v>
+      </c>
+      <c r="D22" s="60">
+        <v>0</v>
+      </c>
       <c r="E22" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -25889,11 +25991,15 @@
       <c r="B23" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="60"/>
+      <c r="C23" s="59" t="s">
+        <v>296</v>
+      </c>
+      <c r="D23" s="60">
+        <v>47</v>
+      </c>
       <c r="E23" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1082880</v>
       </c>
       <c r="F23" s="61">
         <v>23040</v>
@@ -25954,8 +26060,12 @@
       <c r="B24" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="60"/>
+      <c r="C24" s="59" t="s">
+        <v>296</v>
+      </c>
+      <c r="D24" s="60">
+        <v>0</v>
+      </c>
       <c r="E24" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -26019,11 +26129,15 @@
       <c r="B25" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="60"/>
+      <c r="C25" s="59" t="s">
+        <v>297</v>
+      </c>
+      <c r="D25" s="60">
+        <v>47</v>
+      </c>
       <c r="E25" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1006270</v>
       </c>
       <c r="F25" s="61">
         <v>21410</v>
@@ -26084,8 +26198,12 @@
       <c r="B26" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="59"/>
-      <c r="D26" s="60"/>
+      <c r="C26" s="59" t="s">
+        <v>297</v>
+      </c>
+      <c r="D26" s="60">
+        <v>0</v>
+      </c>
       <c r="E26" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -26149,11 +26267,15 @@
       <c r="B27" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="60"/>
+      <c r="C27" s="59" t="s">
+        <v>298</v>
+      </c>
+      <c r="D27" s="60">
+        <v>47</v>
+      </c>
       <c r="E27" s="40">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1069720</v>
       </c>
       <c r="F27" s="61">
         <v>22760</v>
@@ -26210,8 +26332,12 @@
       <c r="B28" s="58" t="s">
         <v>254</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="60"/>
+      <c r="C28" s="59" t="s">
+        <v>298</v>
+      </c>
+      <c r="D28" s="60">
+        <v>0</v>
+      </c>
       <c r="E28" s="40">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -27436,13 +27562,13 @@
       <c r="V54" s="160"/>
     </row>
     <row r="55" spans="1:24" s="161" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A55" s="507" t="s">
+      <c r="A55" s="508" t="s">
         <v>41</v>
       </c>
       <c r="B55" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="472" t="s">
+      <c r="C55" s="482" t="s">
         <v>232</v>
       </c>
       <c r="D55" s="439"/>
@@ -27453,7 +27579,7 @@
       <c r="G55" s="152">
         <v>44627</v>
       </c>
-      <c r="H55" s="510" t="s">
+      <c r="H55" s="511" t="s">
         <v>233</v>
       </c>
       <c r="I55" s="151">
@@ -27472,10 +27598,10 @@
         <f t="shared" si="1"/>
         <v>18886.399999999998</v>
       </c>
-      <c r="O55" s="468" t="s">
+      <c r="O55" s="488" t="s">
         <v>59</v>
       </c>
-      <c r="P55" s="462">
+      <c r="P55" s="494">
         <v>44645</v>
       </c>
       <c r="Q55" s="128"/>
@@ -27486,11 +27612,11 @@
       <c r="V55" s="160"/>
     </row>
     <row r="56" spans="1:24" s="161" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="509"/>
+      <c r="A56" s="510"/>
       <c r="B56" s="438" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="473"/>
+      <c r="C56" s="483"/>
       <c r="D56" s="440"/>
       <c r="E56" s="60"/>
       <c r="F56" s="151">
@@ -27499,7 +27625,7 @@
       <c r="G56" s="152">
         <v>44627</v>
       </c>
-      <c r="H56" s="511"/>
+      <c r="H56" s="512"/>
       <c r="I56" s="151">
         <v>967</v>
       </c>
@@ -27516,8 +27642,8 @@
         <f t="shared" si="1"/>
         <v>92832</v>
       </c>
-      <c r="O56" s="469"/>
-      <c r="P56" s="463"/>
+      <c r="O56" s="489"/>
+      <c r="P56" s="495"/>
       <c r="Q56" s="164"/>
       <c r="R56" s="158"/>
       <c r="S56" s="92"/>
@@ -27688,13 +27814,13 @@
       <c r="V61" s="54"/>
     </row>
     <row r="62" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A62" s="512" t="s">
+      <c r="A62" s="513" t="s">
         <v>106</v>
       </c>
       <c r="B62" s="178" t="s">
         <v>243</v>
       </c>
-      <c r="C62" s="514" t="s">
+      <c r="C62" s="515" t="s">
         <v>244</v>
       </c>
       <c r="D62" s="168"/>
@@ -27705,7 +27831,7 @@
       <c r="G62" s="152">
         <v>44622</v>
       </c>
-      <c r="H62" s="516">
+      <c r="H62" s="517">
         <v>37162</v>
       </c>
       <c r="I62" s="151">
@@ -27724,10 +27850,10 @@
         <f t="shared" si="1"/>
         <v>7782.5999999999995</v>
       </c>
-      <c r="O62" s="468" t="s">
+      <c r="O62" s="488" t="s">
         <v>61</v>
       </c>
-      <c r="P62" s="462">
+      <c r="P62" s="494">
         <v>44643</v>
       </c>
       <c r="Q62" s="164"/>
@@ -27738,11 +27864,11 @@
       <c r="V62" s="54"/>
     </row>
     <row r="63" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A63" s="513"/>
+      <c r="A63" s="514"/>
       <c r="B63" s="178" t="s">
         <v>245</v>
       </c>
-      <c r="C63" s="515"/>
+      <c r="C63" s="516"/>
       <c r="D63" s="168"/>
       <c r="E63" s="60"/>
       <c r="F63" s="151">
@@ -27751,7 +27877,7 @@
       <c r="G63" s="152">
         <v>44622</v>
       </c>
-      <c r="H63" s="517"/>
+      <c r="H63" s="518"/>
       <c r="I63" s="151">
         <v>204.8</v>
       </c>
@@ -27768,8 +27894,8 @@
         <f t="shared" si="1"/>
         <v>16998.400000000001</v>
       </c>
-      <c r="O63" s="469"/>
-      <c r="P63" s="463"/>
+      <c r="O63" s="489"/>
+      <c r="P63" s="495"/>
       <c r="Q63" s="164"/>
       <c r="R63" s="129"/>
       <c r="S63" s="92"/>
@@ -28248,8 +28374,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O79" s="468"/>
-      <c r="P79" s="482"/>
+      <c r="O79" s="488"/>
+      <c r="P79" s="490"/>
       <c r="Q79" s="164"/>
       <c r="R79" s="129"/>
       <c r="S79" s="180"/>
@@ -28278,8 +28404,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O80" s="469"/>
-      <c r="P80" s="483"/>
+      <c r="O80" s="489"/>
+      <c r="P80" s="491"/>
       <c r="Q80" s="164"/>
       <c r="R80" s="129"/>
       <c r="S80" s="180"/>
@@ -28308,8 +28434,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O81" s="468"/>
-      <c r="P81" s="482"/>
+      <c r="O81" s="488"/>
+      <c r="P81" s="490"/>
       <c r="Q81" s="164"/>
       <c r="R81" s="158"/>
       <c r="S81" s="180"/>
@@ -28341,8 +28467,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O82" s="469"/>
-      <c r="P82" s="483"/>
+      <c r="O82" s="489"/>
+      <c r="P82" s="491"/>
       <c r="Q82" s="164"/>
       <c r="R82" s="158"/>
       <c r="S82" s="180"/>
@@ -28500,8 +28626,8 @@
         <v>0</v>
       </c>
       <c r="K87" s="100"/>
-      <c r="L87" s="484"/>
-      <c r="M87" s="485"/>
+      <c r="L87" s="492"/>
+      <c r="M87" s="493"/>
       <c r="N87" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -28533,8 +28659,8 @@
         <v>0</v>
       </c>
       <c r="K88" s="100"/>
-      <c r="L88" s="484"/>
-      <c r="M88" s="485"/>
+      <c r="L88" s="492"/>
+      <c r="M88" s="493"/>
       <c r="N88" s="48">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -28737,8 +28863,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O94" s="468"/>
-      <c r="P94" s="478"/>
+      <c r="O94" s="488"/>
+      <c r="P94" s="484"/>
       <c r="Q94" s="164"/>
       <c r="R94" s="129"/>
       <c r="S94" s="180"/>
@@ -28770,8 +28896,8 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O95" s="469"/>
-      <c r="P95" s="479"/>
+      <c r="O95" s="489"/>
+      <c r="P95" s="485"/>
       <c r="Q95" s="164"/>
       <c r="R95" s="129"/>
       <c r="S95" s="180"/>
@@ -34163,11 +34289,11 @@
         <f t="shared" si="10"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F259" s="480" t="s">
+      <c r="F259" s="486" t="s">
         <v>26</v>
       </c>
-      <c r="G259" s="480"/>
-      <c r="H259" s="481"/>
+      <c r="G259" s="486"/>
+      <c r="H259" s="487"/>
       <c r="I259" s="317">
         <f>SUM(I4:I258)</f>
         <v>515771.39999999997</v>
@@ -34741,6 +34867,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="O94:O95"/>
+    <mergeCell ref="P94:P95"/>
+    <mergeCell ref="F259:H259"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="S1:T2"/>
     <mergeCell ref="W1:X1"/>
@@ -34756,13 +34889,6 @@
     <mergeCell ref="H62:H63"/>
     <mergeCell ref="O62:O63"/>
     <mergeCell ref="P62:P63"/>
-    <mergeCell ref="O94:O95"/>
-    <mergeCell ref="P94:P95"/>
-    <mergeCell ref="F259:H259"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>